<commit_message>
- fixed incorrectly reported compositions, temperature, and processing from `10.1016/j.jallcom.2016.06.161`
</commit_message>
<xml_diff>
--- a/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
+++ b/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05A07EE-77AE-BD4E-B686-7F6EA054212E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EDF8B3-0D3D-774B-BD99-C9298D059E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="218">
   <si>
     <t>Name:</t>
   </si>
@@ -613,9 +613,6 @@
     <t>Cr16.8 Mo17.6 Nb17.9 Ta18.5 V11.4 W17.8</t>
   </si>
   <si>
-    <t>Mo98.57 Ti1.16 Zr0.004 Co0.24 S0.29</t>
-  </si>
-  <si>
     <t>Mo25 Nb25 Ta25 V25</t>
   </si>
   <si>
@@ -680,6 +677,45 @@
   </si>
   <si>
     <t>Nb Ta Ti V W</t>
+  </si>
+  <si>
+    <t>Mo98.74 Ti0.996 Zr0.104 C0.159</t>
+  </si>
+  <si>
+    <t>SPS</t>
+  </si>
+  <si>
+    <t>1723K SPS for 300s at 40MPa</t>
+  </si>
+  <si>
+    <t>1773K SPS for 300s at 40MPa</t>
+  </si>
+  <si>
+    <t>1798K SPS for 300s at 40MPa</t>
+  </si>
+  <si>
+    <t>1823K SPS for 300s at 40MPa</t>
+  </si>
+  <si>
+    <t>1848K SPS for 300s at 40MPa</t>
+  </si>
+  <si>
+    <t>1848K SPS for 150s at 40MPa</t>
+  </si>
+  <si>
+    <t>1723K SPS for 150s at 40MPa</t>
+  </si>
+  <si>
+    <t>1723K SPS for 150s at 60MPa</t>
+  </si>
+  <si>
+    <t>1723K SPS for 150s at 70MPa</t>
+  </si>
+  <si>
+    <t>1723K SPS for 150s at 80MPa</t>
+  </si>
+  <si>
+    <t>1973K SPS for 150s at 80MPa</t>
   </si>
 </sst>
 </file>
@@ -862,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -971,6 +1007,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1259,8 +1297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C93" sqref="C93"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1294,14 +1332,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="45"/>
       <c r="F2" s="43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -1318,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" s="45"/>
       <c r="E3" s="45"/>
@@ -1570,7 +1608,7 @@
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>123</v>
@@ -1610,7 +1648,7 @@
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>123</v>
@@ -1650,7 +1688,7 @@
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>123</v>
@@ -1690,7 +1728,7 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>123</v>
@@ -1730,7 +1768,7 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>123</v>
@@ -1770,7 +1808,7 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>123</v>
@@ -1810,7 +1848,7 @@
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>123</v>
@@ -1850,7 +1888,7 @@
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>123</v>
@@ -1889,7 +1927,7 @@
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>123</v>
@@ -1928,7 +1966,7 @@
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>123</v>
@@ -1967,7 +2005,7 @@
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>123</v>
@@ -2006,7 +2044,7 @@
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>123</v>
@@ -2045,7 +2083,7 @@
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>123</v>
@@ -2084,7 +2122,7 @@
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>123</v>
@@ -2123,7 +2161,7 @@
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>123</v>
@@ -2162,7 +2200,7 @@
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>123</v>
@@ -2201,7 +2239,7 @@
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>123</v>
@@ -2240,7 +2278,7 @@
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>123</v>
@@ -2279,7 +2317,7 @@
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>123</v>
@@ -2318,7 +2356,7 @@
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>123</v>
@@ -2357,7 +2395,7 @@
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>123</v>
@@ -2396,7 +2434,7 @@
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>123</v>
@@ -2435,7 +2473,7 @@
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>123</v>
@@ -2474,7 +2512,7 @@
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>123</v>
@@ -2513,7 +2551,7 @@
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>123</v>
@@ -2552,7 +2590,7 @@
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>123</v>
@@ -2588,7 +2626,7 @@
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>123</v>
@@ -2624,7 +2662,7 @@
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>123</v>
@@ -2660,7 +2698,7 @@
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>123</v>
@@ -2695,7 +2733,7 @@
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>123</v>
@@ -2730,7 +2768,7 @@
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>123</v>
@@ -2765,7 +2803,7 @@
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>123</v>
@@ -2799,7 +2837,7 @@
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>123</v>
@@ -2835,7 +2873,7 @@
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>123</v>
@@ -2871,7 +2909,7 @@
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>123</v>
@@ -2907,7 +2945,7 @@
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>123</v>
@@ -2943,7 +2981,7 @@
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>123</v>
@@ -2979,7 +3017,7 @@
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>123</v>
@@ -3015,7 +3053,7 @@
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>123</v>
@@ -3051,7 +3089,7 @@
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>123</v>
@@ -3087,7 +3125,7 @@
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>123</v>
@@ -3123,7 +3161,7 @@
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>123</v>
@@ -3156,7 +3194,7 @@
       <c r="C52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>123</v>
@@ -3189,7 +3227,7 @@
       <c r="C53" s="20"/>
       <c r="E53" s="20"/>
       <c r="F53" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>123</v>
@@ -3222,7 +3260,7 @@
       <c r="C54" s="20"/>
       <c r="E54" s="20"/>
       <c r="F54" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>123</v>
@@ -3255,7 +3293,7 @@
       <c r="C55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>123</v>
@@ -3288,7 +3326,7 @@
       <c r="C56" s="20"/>
       <c r="E56" s="20"/>
       <c r="F56" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G56" s="20" t="s">
         <v>123</v>
@@ -3321,7 +3359,7 @@
       <c r="C57" s="20"/>
       <c r="E57" s="20"/>
       <c r="F57" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G57" s="20" t="s">
         <v>123</v>
@@ -3357,7 +3395,7 @@
       </c>
       <c r="E58" s="20"/>
       <c r="F58" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>123</v>
@@ -3392,7 +3430,7 @@
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>123</v>
@@ -3427,7 +3465,7 @@
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G60" s="20" t="s">
         <v>123</v>
@@ -3462,7 +3500,7 @@
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G61" s="20" t="s">
         <v>123</v>
@@ -3499,7 +3537,7 @@
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G62" s="20" t="s">
         <v>123</v>
@@ -3538,7 +3576,7 @@
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G63" s="20" t="s">
         <v>123</v>
@@ -3577,7 +3615,7 @@
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G64" s="20" t="s">
         <v>123</v>
@@ -3616,7 +3654,7 @@
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G65" s="20" t="s">
         <v>123</v>
@@ -3655,7 +3693,7 @@
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>123</v>
@@ -3692,7 +3730,7 @@
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G67" s="20" t="s">
         <v>123</v>
@@ -3729,7 +3767,7 @@
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G68" s="20" t="s">
         <v>123</v>
@@ -3766,7 +3804,7 @@
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G69" s="20" t="s">
         <v>123</v>
@@ -3803,7 +3841,7 @@
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G70" s="20" t="s">
         <v>123</v>
@@ -3840,7 +3878,7 @@
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>123</v>
@@ -3877,7 +3915,7 @@
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G72" s="20" t="s">
         <v>123</v>
@@ -3914,7 +3952,7 @@
       </c>
       <c r="E73" s="20"/>
       <c r="F73" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G73" s="20" t="s">
         <v>123</v>
@@ -3946,7 +3984,7 @@
       <c r="C74" s="20"/>
       <c r="E74" s="20"/>
       <c r="F74" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G74" s="20" t="s">
         <v>123</v>
@@ -3977,7 +4015,7 @@
       <c r="C75" s="20"/>
       <c r="E75" s="20"/>
       <c r="F75" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G75" s="20" t="s">
         <v>123</v>
@@ -4008,7 +4046,7 @@
       <c r="C76" s="20"/>
       <c r="E76" s="20"/>
       <c r="F76" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G76" s="20" t="s">
         <v>123</v>
@@ -4041,7 +4079,7 @@
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G77" s="20" t="s">
         <v>123</v>
@@ -4076,7 +4114,7 @@
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>123</v>
@@ -4111,7 +4149,7 @@
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G79" s="20" t="s">
         <v>123</v>
@@ -4146,7 +4184,7 @@
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G80" s="20" t="s">
         <v>123</v>
@@ -4182,7 +4220,7 @@
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G81" s="20" t="s">
         <v>123</v>
@@ -4218,7 +4256,7 @@
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G82" s="20" t="s">
         <v>123</v>
@@ -4254,7 +4292,7 @@
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G83" s="20" t="s">
         <v>123</v>
@@ -4289,7 +4327,7 @@
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G84" s="20" t="s">
         <v>123</v>
@@ -4324,7 +4362,7 @@
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>123</v>
@@ -4359,7 +4397,7 @@
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G86" s="20" t="s">
         <v>123</v>
@@ -4394,7 +4432,7 @@
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G87" s="20" t="s">
         <v>123</v>
@@ -4429,7 +4467,7 @@
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G88" s="20" t="s">
         <v>123</v>
@@ -4457,14 +4495,14 @@
         <v>80</v>
       </c>
       <c r="B89" s="49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C89" s="20" t="s">
         <v>117</v>
       </c>
       <c r="E89" s="20"/>
       <c r="F89" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G89" s="20" t="s">
         <v>123</v>
@@ -4492,14 +4530,14 @@
         <v>81</v>
       </c>
       <c r="B90" s="49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C90" s="20" t="s">
         <v>117</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G90" s="20" t="s">
         <v>123</v>
@@ -4527,14 +4565,14 @@
         <v>82</v>
       </c>
       <c r="B91" s="49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C91" s="20" t="s">
         <v>117</v>
       </c>
       <c r="E91" s="20"/>
       <c r="F91" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G91" s="20" t="s">
         <v>123</v>
@@ -4568,11 +4606,11 @@
         <v>117</v>
       </c>
       <c r="D92" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E92" s="20"/>
       <c r="F92" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G92" s="20" t="s">
         <v>123</v>
@@ -4604,11 +4642,11 @@
         <v>90</v>
       </c>
       <c r="D93" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E93" s="20"/>
       <c r="F93" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G93" s="20" t="s">
         <v>123</v>
@@ -4640,11 +4678,11 @@
         <v>91</v>
       </c>
       <c r="D94" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E94" s="20"/>
       <c r="F94" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G94" s="20" t="s">
         <v>123</v>
@@ -4672,22 +4710,27 @@
       <c r="A95" s="3">
         <v>86</v>
       </c>
-      <c r="B95" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D95" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E95" s="20"/>
+      <c r="B95" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C95" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D95" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E95" s="51" t="s">
+        <v>207</v>
+      </c>
       <c r="F95" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G95" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H95" s="22"/>
-      <c r="I95" s="23">
-        <v>1723</v>
+      <c r="I95" s="3">
+        <v>298</v>
       </c>
       <c r="J95" s="19">
         <v>1910000000</v>
@@ -4707,22 +4750,27 @@
       <c r="A96" s="3">
         <v>87</v>
       </c>
-      <c r="B96" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D96" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E96" s="20"/>
+      <c r="B96" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C96" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D96" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E96" s="51" t="s">
+        <v>208</v>
+      </c>
       <c r="F96" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G96" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H96" s="22"/>
-      <c r="I96" s="23">
-        <v>1773</v>
+      <c r="I96" s="3">
+        <v>298</v>
       </c>
       <c r="J96" s="19">
         <v>1890000000</v>
@@ -4742,22 +4790,27 @@
       <c r="A97" s="3">
         <v>88</v>
       </c>
-      <c r="B97" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D97" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E97" s="20"/>
+      <c r="B97" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C97" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D97" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E97" s="51" t="s">
+        <v>209</v>
+      </c>
       <c r="F97" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G97" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H97" s="22"/>
-      <c r="I97" s="23">
-        <v>1798</v>
+      <c r="I97" s="3">
+        <v>298</v>
       </c>
       <c r="J97" s="19">
         <v>1840000000</v>
@@ -4777,22 +4830,27 @@
       <c r="A98" s="3">
         <v>89</v>
       </c>
-      <c r="B98" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D98" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E98" s="20"/>
+      <c r="B98" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C98" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D98" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E98" s="51" t="s">
+        <v>210</v>
+      </c>
       <c r="F98" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G98" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H98" s="22"/>
-      <c r="I98" s="23">
-        <v>1823</v>
+      <c r="I98" s="3">
+        <v>298</v>
       </c>
       <c r="J98" s="19">
         <v>1820000000</v>
@@ -4812,22 +4870,27 @@
       <c r="A99" s="3">
         <v>90</v>
       </c>
-      <c r="B99" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D99" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E99" s="20"/>
+      <c r="B99" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C99" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D99" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E99" s="51" t="s">
+        <v>211</v>
+      </c>
       <c r="F99" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G99" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H99" s="22"/>
-      <c r="I99" s="23">
-        <v>1848</v>
+      <c r="I99" s="3">
+        <v>298</v>
       </c>
       <c r="J99" s="19">
         <v>1850000000</v>
@@ -4847,22 +4910,27 @@
       <c r="A100" s="3">
         <v>91</v>
       </c>
-      <c r="B100" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D100" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E100" s="20"/>
+      <c r="B100" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C100" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D100" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E100" s="51" t="s">
+        <v>212</v>
+      </c>
       <c r="F100" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G100" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H100" s="22"/>
-      <c r="I100" s="23">
-        <v>1848</v>
+      <c r="I100" s="3">
+        <v>298</v>
       </c>
       <c r="J100" s="19">
         <v>1810000000</v>
@@ -4882,22 +4950,27 @@
       <c r="A101" s="3">
         <v>92</v>
       </c>
-      <c r="B101" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D101" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E101" s="20"/>
+      <c r="B101" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C101" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D101" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E101" s="51" t="s">
+        <v>213</v>
+      </c>
       <c r="F101" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G101" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H101" s="22"/>
-      <c r="I101" s="23">
-        <v>1723</v>
+      <c r="I101" s="3">
+        <v>298</v>
       </c>
       <c r="J101" s="19">
         <v>1750000000</v>
@@ -4917,22 +4990,27 @@
       <c r="A102" s="3">
         <v>93</v>
       </c>
-      <c r="B102" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D102" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E102" s="20"/>
+      <c r="B102" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C102" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D102" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E102" s="51" t="s">
+        <v>214</v>
+      </c>
       <c r="F102" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G102" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H102" s="22"/>
-      <c r="I102" s="23">
-        <v>1723</v>
+      <c r="I102" s="3">
+        <v>298</v>
       </c>
       <c r="J102" s="19">
         <v>1920000000</v>
@@ -4952,22 +5030,27 @@
       <c r="A103" s="3">
         <v>94</v>
       </c>
-      <c r="B103" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D103" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E103" s="20"/>
+      <c r="B103" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C103" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D103" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E103" s="51" t="s">
+        <v>215</v>
+      </c>
       <c r="F103" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G103" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H103" s="22"/>
-      <c r="I103" s="23">
-        <v>1723</v>
+      <c r="I103" s="3">
+        <v>298</v>
       </c>
       <c r="J103" s="19">
         <v>1950000000</v>
@@ -4987,22 +5070,27 @@
       <c r="A104" s="3">
         <v>95</v>
       </c>
-      <c r="B104" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D104" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E104" s="20"/>
+      <c r="B104" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C104" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D104" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E104" s="51" t="s">
+        <v>216</v>
+      </c>
       <c r="F104" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G104" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H104" s="22"/>
-      <c r="I104" s="23">
-        <v>1723</v>
+      <c r="I104" s="3">
+        <v>298</v>
       </c>
       <c r="J104" s="19">
         <v>2040000000</v>
@@ -5022,22 +5110,27 @@
       <c r="A105" s="3">
         <v>96</v>
       </c>
-      <c r="B105" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D105" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E105" s="20"/>
+      <c r="B105" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C105" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="D105" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="E105" s="51" t="s">
+        <v>217</v>
+      </c>
       <c r="F105" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G105" s="20" t="s">
         <v>123</v>
       </c>
       <c r="H105" s="22"/>
-      <c r="I105" s="23">
-        <v>1973</v>
+      <c r="I105" s="3">
+        <v>298</v>
       </c>
       <c r="J105" s="19">
         <v>1980000000</v>
@@ -5065,7 +5158,7 @@
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G106" s="20" t="s">
         <v>123</v>
@@ -5099,7 +5192,7 @@
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G107" s="20" t="s">
         <v>123</v>
@@ -5133,7 +5226,7 @@
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G108" s="20" t="s">
         <v>123</v>
@@ -5167,7 +5260,7 @@
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G109" s="20" t="s">
         <v>123</v>
@@ -5204,7 +5297,7 @@
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G110" s="20" t="s">
         <v>123</v>
@@ -5231,7 +5324,7 @@
         <v>102</v>
       </c>
       <c r="B111" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>117</v>
@@ -5241,7 +5334,7 @@
       </c>
       <c r="E111" s="20"/>
       <c r="F111" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G111" s="20" t="s">
         <v>123</v>
@@ -5278,7 +5371,7 @@
       </c>
       <c r="E112" s="20"/>
       <c r="F112" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G112" s="20" t="s">
         <v>123</v>
@@ -5315,7 +5408,7 @@
       </c>
       <c r="E113" s="20"/>
       <c r="F113" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G113" s="20" t="s">
         <v>123</v>
@@ -5352,7 +5445,7 @@
       </c>
       <c r="E114" s="20"/>
       <c r="F114" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G114" s="20" t="s">
         <v>123</v>
@@ -5389,7 +5482,7 @@
       </c>
       <c r="E115" s="20"/>
       <c r="F115" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G115" s="20" t="s">
         <v>123</v>
@@ -5426,7 +5519,7 @@
       </c>
       <c r="E116" s="20"/>
       <c r="F116" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G116" s="20" t="s">
         <v>123</v>
@@ -5463,7 +5556,7 @@
       </c>
       <c r="E117" s="20"/>
       <c r="F117" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G117" s="20" t="s">
         <v>123</v>
@@ -5500,7 +5593,7 @@
       </c>
       <c r="E118" s="20"/>
       <c r="F118" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G118" s="20" t="s">
         <v>123</v>
@@ -5537,7 +5630,7 @@
       </c>
       <c r="E119" s="20"/>
       <c r="F119" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G119" s="20" t="s">
         <v>123</v>
@@ -5574,7 +5667,7 @@
       </c>
       <c r="E120" s="20"/>
       <c r="F120" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G120" s="20" t="s">
         <v>123</v>
@@ -5611,7 +5704,7 @@
       </c>
       <c r="E121" s="20"/>
       <c r="F121" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G121" s="20" t="s">
         <v>123</v>
@@ -5644,11 +5737,11 @@
         <v>117</v>
       </c>
       <c r="D122" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E122" s="20"/>
       <c r="F122" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G122" s="20" t="s">
         <v>123</v>
@@ -5682,11 +5775,11 @@
         <v>117</v>
       </c>
       <c r="D123" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E123" s="20"/>
       <c r="F123" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G123" s="20" t="s">
         <v>123</v>
@@ -5720,11 +5813,11 @@
         <v>117</v>
       </c>
       <c r="D124" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E124" s="20"/>
       <c r="F124" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G124" s="20" t="s">
         <v>123</v>
@@ -5758,11 +5851,11 @@
         <v>117</v>
       </c>
       <c r="D125" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E125" s="20"/>
       <c r="F125" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G125" s="20" t="s">
         <v>123</v>
@@ -5800,7 +5893,7 @@
       </c>
       <c r="E126" s="20"/>
       <c r="F126" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G126" s="20" t="s">
         <v>123</v>
@@ -5833,11 +5926,11 @@
         <v>117</v>
       </c>
       <c r="D127" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E127" s="20"/>
       <c r="F127" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G127" s="20" t="s">
         <v>123</v>
@@ -5872,11 +5965,11 @@
         <v>117</v>
       </c>
       <c r="D128" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E128" s="20"/>
       <c r="F128" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G128" s="20" t="s">
         <v>123</v>
@@ -5911,11 +6004,11 @@
         <v>117</v>
       </c>
       <c r="D129" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E129" s="20"/>
       <c r="F129" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G129" s="20" t="s">
         <v>123</v>
@@ -5944,7 +6037,7 @@
         <v>121</v>
       </c>
       <c r="B130" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>117</v>
@@ -5954,7 +6047,7 @@
       </c>
       <c r="E130" s="20"/>
       <c r="F130" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G130" s="20" t="s">
         <v>123</v>
@@ -5983,14 +6076,14 @@
         <v>122</v>
       </c>
       <c r="B131" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D131" s="3" t="s">
         <v>120</v>
       </c>
       <c r="E131" s="20"/>
       <c r="F131" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G131" s="20" t="s">
         <v>123</v>
@@ -6019,14 +6112,14 @@
         <v>123</v>
       </c>
       <c r="B132" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>120</v>
       </c>
       <c r="E132" s="20"/>
       <c r="F132" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G132" s="20" t="s">
         <v>123</v>
@@ -6055,14 +6148,14 @@
         <v>124</v>
       </c>
       <c r="B133" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>120</v>
       </c>
       <c r="E133" s="20"/>
       <c r="F133" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G133" s="20" t="s">
         <v>123</v>
@@ -6098,7 +6191,7 @@
       </c>
       <c r="E134" s="20"/>
       <c r="F134" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G134" s="20" t="s">
         <v>123</v>
@@ -6133,7 +6226,7 @@
       </c>
       <c r="E135" s="20"/>
       <c r="F135" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G135" s="20" t="s">
         <v>123</v>
@@ -6168,7 +6261,7 @@
       </c>
       <c r="E136" s="20"/>
       <c r="F136" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G136" s="20" t="s">
         <v>123</v>
@@ -6203,7 +6296,7 @@
       </c>
       <c r="E137" s="20"/>
       <c r="F137" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G137" s="20" t="s">
         <v>123</v>
@@ -6238,7 +6331,7 @@
       </c>
       <c r="E138" s="20"/>
       <c r="F138" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G138" s="20" t="s">
         <v>123</v>
@@ -6273,7 +6366,7 @@
       </c>
       <c r="E139" s="20"/>
       <c r="F139" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G139" s="20" t="s">
         <v>123</v>
@@ -6308,7 +6401,7 @@
       </c>
       <c r="E140" s="20"/>
       <c r="F140" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G140" s="20" t="s">
         <v>123</v>
@@ -6343,7 +6436,7 @@
       </c>
       <c r="E141" s="20"/>
       <c r="F141" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G141" s="20" t="s">
         <v>123</v>
@@ -6375,7 +6468,7 @@
       </c>
       <c r="E142" s="20"/>
       <c r="F142" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G142" s="20" t="s">
         <v>123</v>
@@ -6407,7 +6500,7 @@
       </c>
       <c r="E143" s="20"/>
       <c r="F143" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G143" s="20" t="s">
         <v>123</v>
@@ -6433,17 +6526,17 @@
         <v>135</v>
       </c>
       <c r="B144" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D144" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E144" s="20"/>
       <c r="F144" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G144" s="20" t="s">
         <v>123</v>
@@ -6472,17 +6565,17 @@
         <v>136</v>
       </c>
       <c r="B145" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D145" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E145" s="20"/>
       <c r="F145" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G145" s="20" t="s">
         <v>123</v>
@@ -6511,17 +6604,17 @@
         <v>137</v>
       </c>
       <c r="B146" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D146" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E146" s="20"/>
       <c r="F146" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G146" s="20" t="s">
         <v>123</v>
@@ -6550,17 +6643,17 @@
         <v>138</v>
       </c>
       <c r="B147" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D147" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E147" s="20"/>
       <c r="F147" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G147" s="20" t="s">
         <v>123</v>
@@ -6589,17 +6682,17 @@
         <v>139</v>
       </c>
       <c r="B148" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D148" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E148" s="20"/>
       <c r="F148" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G148" s="20" t="s">
         <v>123</v>
@@ -6628,17 +6721,17 @@
         <v>140</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D149" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E149" s="20"/>
       <c r="F149" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G149" s="20" t="s">
         <v>123</v>
@@ -6667,17 +6760,17 @@
         <v>141</v>
       </c>
       <c r="B150" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D150" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E150" s="20"/>
       <c r="F150" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G150" s="20" t="s">
         <v>123</v>
@@ -6706,17 +6799,17 @@
         <v>142</v>
       </c>
       <c r="B151" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>121</v>
       </c>
       <c r="D151" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E151" s="20"/>
       <c r="F151" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G151" s="20" t="s">
         <v>123</v>
@@ -6752,7 +6845,7 @@
       </c>
       <c r="E152" s="20"/>
       <c r="F152" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G152" s="20" t="s">
         <v>123</v>
@@ -6786,7 +6879,7 @@
       </c>
       <c r="E153" s="20"/>
       <c r="F153" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G153" s="20" t="s">
         <v>123</v>
@@ -6818,11 +6911,11 @@
         <v>111</v>
       </c>
       <c r="D154" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E154" s="20"/>
       <c r="F154" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G154" s="20" t="s">
         <v>123</v>
@@ -6854,11 +6947,11 @@
         <v>111</v>
       </c>
       <c r="D155" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E155" s="20"/>
       <c r="F155" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G155" s="20" t="s">
         <v>123</v>
@@ -6894,7 +6987,7 @@
       </c>
       <c r="E156" s="20"/>
       <c r="F156" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G156" s="20" t="s">
         <v>123</v>
@@ -6928,7 +7021,7 @@
       </c>
       <c r="E157" s="20"/>
       <c r="F157" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G157" s="20" t="s">
         <v>123</v>
@@ -6960,11 +7053,11 @@
         <v>112</v>
       </c>
       <c r="D158" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E158" s="20"/>
       <c r="F158" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G158" s="20" t="s">
         <v>123</v>
@@ -6996,11 +7089,11 @@
         <v>112</v>
       </c>
       <c r="D159" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E159" s="20"/>
       <c r="F159" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G159" s="20" t="s">
         <v>123</v>
@@ -7036,7 +7129,7 @@
       </c>
       <c r="E160" s="20"/>
       <c r="F160" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G160" s="20" t="s">
         <v>123</v>
@@ -7070,7 +7163,7 @@
       </c>
       <c r="E161" s="20"/>
       <c r="F161" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G161" s="20" t="s">
         <v>123</v>
@@ -7104,7 +7197,7 @@
       </c>
       <c r="E162" s="20"/>
       <c r="F162" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G162" s="20" t="s">
         <v>123</v>
@@ -7138,7 +7231,7 @@
       </c>
       <c r="E163" s="20"/>
       <c r="F163" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G163" s="20" t="s">
         <v>123</v>
@@ -7172,7 +7265,7 @@
       </c>
       <c r="E164" s="20"/>
       <c r="F164" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G164" s="20" t="s">
         <v>123</v>
@@ -7199,7 +7292,7 @@
         <v>156</v>
       </c>
       <c r="B165" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>117</v>
@@ -7209,7 +7302,7 @@
       </c>
       <c r="E165" s="20"/>
       <c r="F165" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G165" s="20" t="s">
         <v>123</v>
@@ -7236,17 +7329,17 @@
         <v>157</v>
       </c>
       <c r="B166" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="C166" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="C166" s="36" t="s">
-        <v>194</v>
-      </c>
       <c r="D166" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E166" s="20"/>
       <c r="F166" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G166" s="20" t="s">
         <v>123</v>
@@ -7275,19 +7368,19 @@
         <v>158</v>
       </c>
       <c r="B167" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C167" s="36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D167" s="36" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E167" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F167" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G167" s="20" t="s">
         <v>123</v>
@@ -7316,19 +7409,19 @@
         <v>159</v>
       </c>
       <c r="B168" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C168" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="D168" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="E168" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="D168" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E168" s="31" t="s">
-        <v>200</v>
-      </c>
       <c r="F168" s="31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G168" s="20" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
- fixed incorrectly reported compositions, temperature, and processing from `10.3390/met9010076`
</commit_message>
<xml_diff>
--- a/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
+++ b/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95A6D6E-E08C-2648-8356-D4BB80FB5401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F247196-A11D-AB4C-B96E-5FD796574589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="221">
   <si>
     <t>Name:</t>
   </si>
@@ -719,6 +719,12 @@
   </si>
   <si>
     <t>Ta87.4 W11.2 (TiC)0.7</t>
+  </si>
+  <si>
+    <t>1523K sintering temperature</t>
+  </si>
+  <si>
+    <t>1573K sintering temperature</t>
   </si>
 </sst>
 </file>
@@ -1307,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H84" sqref="H84"/>
+    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -6544,13 +6550,15 @@
       <c r="B144" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="C144" s="3" t="s">
-        <v>119</v>
+      <c r="C144" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="D144" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E144" s="20"/>
+      <c r="E144" s="51" t="s">
+        <v>219</v>
+      </c>
       <c r="F144" s="31" t="s">
         <v>198</v>
       </c>
@@ -6558,8 +6566,8 @@
         <v>121</v>
       </c>
       <c r="H144" s="22"/>
-      <c r="I144" s="23">
-        <v>1523</v>
+      <c r="I144" s="3">
+        <v>298</v>
       </c>
       <c r="J144" s="19">
         <f>341*9807000</f>
@@ -6583,13 +6591,15 @@
       <c r="B145" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="C145" s="3" t="s">
-        <v>119</v>
+      <c r="C145" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="D145" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E145" s="20"/>
+      <c r="E145" s="51" t="s">
+        <v>219</v>
+      </c>
       <c r="F145" s="31" t="s">
         <v>198</v>
       </c>
@@ -6597,8 +6607,8 @@
         <v>121</v>
       </c>
       <c r="H145" s="22"/>
-      <c r="I145" s="23">
-        <v>1523</v>
+      <c r="I145" s="3">
+        <v>298</v>
       </c>
       <c r="J145" s="19">
         <f>338*9807000</f>
@@ -6622,13 +6632,15 @@
       <c r="B146" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="C146" s="3" t="s">
-        <v>119</v>
+      <c r="C146" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="D146" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E146" s="20"/>
+      <c r="E146" s="51" t="s">
+        <v>219</v>
+      </c>
       <c r="F146" s="31" t="s">
         <v>198</v>
       </c>
@@ -6636,8 +6648,8 @@
         <v>121</v>
       </c>
       <c r="H146" s="22"/>
-      <c r="I146" s="23">
-        <v>1523</v>
+      <c r="I146" s="3">
+        <v>298</v>
       </c>
       <c r="J146" s="19">
         <f>340*9807000</f>
@@ -6661,13 +6673,15 @@
       <c r="B147" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="C147" s="3" t="s">
-        <v>119</v>
+      <c r="C147" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="D147" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E147" s="20"/>
+      <c r="E147" s="51" t="s">
+        <v>219</v>
+      </c>
       <c r="F147" s="31" t="s">
         <v>198</v>
       </c>
@@ -6675,8 +6689,8 @@
         <v>121</v>
       </c>
       <c r="H147" s="22"/>
-      <c r="I147" s="23">
-        <v>1523</v>
+      <c r="I147" s="3">
+        <v>298</v>
       </c>
       <c r="J147" s="19">
         <f>345*9807000</f>
@@ -6700,13 +6714,15 @@
       <c r="B148" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="C148" s="3" t="s">
-        <v>119</v>
+      <c r="C148" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="D148" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E148" s="20"/>
+      <c r="E148" s="51" t="s">
+        <v>220</v>
+      </c>
       <c r="F148" s="31" t="s">
         <v>198</v>
       </c>
@@ -6714,8 +6730,8 @@
         <v>121</v>
       </c>
       <c r="H148" s="22"/>
-      <c r="I148" s="23">
-        <v>1573</v>
+      <c r="I148" s="3">
+        <v>298</v>
       </c>
       <c r="J148" s="19">
         <f>334*9807000</f>
@@ -6739,13 +6755,15 @@
       <c r="B149" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="C149" s="3" t="s">
-        <v>119</v>
+      <c r="C149" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="D149" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E149" s="20"/>
+      <c r="E149" s="51" t="s">
+        <v>220</v>
+      </c>
       <c r="F149" s="31" t="s">
         <v>198</v>
       </c>
@@ -6753,8 +6771,8 @@
         <v>121</v>
       </c>
       <c r="H149" s="22"/>
-      <c r="I149" s="23">
-        <v>1573</v>
+      <c r="I149" s="3">
+        <v>298</v>
       </c>
       <c r="J149" s="19">
         <f>340*9807000</f>
@@ -6778,13 +6796,15 @@
       <c r="B150" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="C150" s="3" t="s">
-        <v>119</v>
+      <c r="C150" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="D150" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E150" s="20"/>
+      <c r="E150" s="51" t="s">
+        <v>220</v>
+      </c>
       <c r="F150" s="31" t="s">
         <v>198</v>
       </c>
@@ -6792,8 +6812,8 @@
         <v>121</v>
       </c>
       <c r="H150" s="22"/>
-      <c r="I150" s="23">
-        <v>1573</v>
+      <c r="I150" s="3">
+        <v>298</v>
       </c>
       <c r="J150" s="19">
         <f>340*9807000</f>
@@ -6817,13 +6837,15 @@
       <c r="B151" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="C151" s="3" t="s">
-        <v>119</v>
+      <c r="C151" s="50" t="s">
+        <v>115</v>
       </c>
       <c r="D151" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="E151" s="20"/>
+      <c r="E151" s="51" t="s">
+        <v>220</v>
+      </c>
       <c r="F151" s="31" t="s">
         <v>198</v>
       </c>
@@ -6831,8 +6853,8 @@
         <v>121</v>
       </c>
       <c r="H151" s="22"/>
-      <c r="I151" s="23">
-        <v>1573</v>
+      <c r="I151" s="3">
+        <v>298</v>
       </c>
       <c r="J151" s="19">
         <f>331*9807000</f>
@@ -6867,7 +6889,9 @@
         <v>121</v>
       </c>
       <c r="H152" s="22"/>
-      <c r="I152" s="23"/>
+      <c r="I152" s="3">
+        <v>298</v>
+      </c>
       <c r="J152" s="19">
         <f>459*9807000</f>
         <v>4501413000</v>

</xml_diff>

<commit_message>
- fixed incorrectly reported temperature, and processing from `10.1016/j.jallcom.2018.12.325`
</commit_message>
<xml_diff>
--- a/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
+++ b/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD3BB3C-CD68-0540-BBE3-FED438962957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61798994-5A46-1D48-B76D-19B7E7AE4003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="222">
   <si>
     <t>Name:</t>
   </si>
@@ -569,18 +569,6 @@
     <t>Mo25 Nb25 Ta25 V25</t>
   </si>
   <si>
-    <t>Nb36.3 Ti32.2 Zr31.5</t>
-  </si>
-  <si>
-    <t>Nb32.1 Ta11.1 Ti28.1 Zr28.7</t>
-  </si>
-  <si>
-    <t>Cr8.7 Nb34.4 Ti29.2 Zr27.7</t>
-  </si>
-  <si>
-    <t>Nb32.6 Re10.3 Ti27.7 Zr29.4</t>
-  </si>
-  <si>
     <t>Ti72.68 Nb23.83 Ta3.49</t>
   </si>
   <si>
@@ -705,6 +693,27 @@
   </si>
   <si>
     <t>SPS for 30min at 30MPa at 1873K</t>
+  </si>
+  <si>
+    <t>NbTiZr</t>
+  </si>
+  <si>
+    <t>Ta10Nb30Ti30Zr30</t>
+  </si>
+  <si>
+    <t>Cr10Nb30Ti30Zr30</t>
+  </si>
+  <si>
+    <t>Re10Nb30Ti30Zr30</t>
+  </si>
+  <si>
+    <t>BCC+C14</t>
+  </si>
+  <si>
+    <t>BCC+C14+C15</t>
+  </si>
+  <si>
+    <t>HIP'd at 1673K for 2h under 276MPa; annealed at 1673K</t>
   </si>
 </sst>
 </file>
@@ -1286,7 +1295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O123" sqref="O123"/>
     </sheetView>
   </sheetViews>
@@ -1321,14 +1330,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D2" s="45" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="45"/>
       <c r="F2" s="43" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G2" s="44"/>
       <c r="H2" s="44"/>
@@ -1345,7 +1354,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D3" s="45"/>
       <c r="E3" s="45"/>
@@ -1597,7 +1606,7 @@
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>119</v>
@@ -1637,7 +1646,7 @@
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>119</v>
@@ -1677,7 +1686,7 @@
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>119</v>
@@ -1717,7 +1726,7 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>119</v>
@@ -1757,7 +1766,7 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>119</v>
@@ -1797,7 +1806,7 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>119</v>
@@ -1837,7 +1846,7 @@
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>119</v>
@@ -1877,7 +1886,7 @@
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>119</v>
@@ -1916,7 +1925,7 @@
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>119</v>
@@ -1955,7 +1964,7 @@
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>119</v>
@@ -1994,7 +2003,7 @@
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>119</v>
@@ -2033,7 +2042,7 @@
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>119</v>
@@ -2072,7 +2081,7 @@
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>119</v>
@@ -2111,7 +2120,7 @@
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>119</v>
@@ -2150,7 +2159,7 @@
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>119</v>
@@ -2189,7 +2198,7 @@
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>119</v>
@@ -2228,7 +2237,7 @@
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>119</v>
@@ -2267,7 +2276,7 @@
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>119</v>
@@ -2306,7 +2315,7 @@
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>119</v>
@@ -2345,7 +2354,7 @@
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>119</v>
@@ -2384,7 +2393,7 @@
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>119</v>
@@ -2423,7 +2432,7 @@
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>119</v>
@@ -2462,7 +2471,7 @@
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>119</v>
@@ -2501,7 +2510,7 @@
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>119</v>
@@ -2540,7 +2549,7 @@
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>119</v>
@@ -2579,7 +2588,7 @@
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>119</v>
@@ -2615,7 +2624,7 @@
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>119</v>
@@ -2651,7 +2660,7 @@
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>119</v>
@@ -2687,7 +2696,7 @@
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>119</v>
@@ -2722,7 +2731,7 @@
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>119</v>
@@ -2757,7 +2766,7 @@
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>119</v>
@@ -2792,7 +2801,7 @@
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>119</v>
@@ -2826,7 +2835,7 @@
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>119</v>
@@ -2862,7 +2871,7 @@
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>119</v>
@@ -2898,7 +2907,7 @@
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>119</v>
@@ -2934,7 +2943,7 @@
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>119</v>
@@ -2970,7 +2979,7 @@
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>119</v>
@@ -3006,7 +3015,7 @@
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>119</v>
@@ -3042,7 +3051,7 @@
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>119</v>
@@ -3078,7 +3087,7 @@
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>119</v>
@@ -3114,7 +3123,7 @@
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>119</v>
@@ -3150,7 +3159,7 @@
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>119</v>
@@ -3183,7 +3192,7 @@
       <c r="C52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>119</v>
@@ -3216,7 +3225,7 @@
       <c r="C53" s="20"/>
       <c r="E53" s="20"/>
       <c r="F53" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>119</v>
@@ -3249,7 +3258,7 @@
       <c r="C54" s="20"/>
       <c r="E54" s="20"/>
       <c r="F54" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>119</v>
@@ -3282,7 +3291,7 @@
       <c r="C55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>119</v>
@@ -3315,7 +3324,7 @@
       <c r="C56" s="20"/>
       <c r="E56" s="20"/>
       <c r="F56" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G56" s="20" t="s">
         <v>119</v>
@@ -3348,7 +3357,7 @@
       <c r="C57" s="20"/>
       <c r="E57" s="20"/>
       <c r="F57" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G57" s="20" t="s">
         <v>119</v>
@@ -3384,7 +3393,7 @@
       </c>
       <c r="E58" s="20"/>
       <c r="F58" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>119</v>
@@ -3419,7 +3428,7 @@
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>119</v>
@@ -3454,7 +3463,7 @@
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G60" s="20" t="s">
         <v>119</v>
@@ -3489,7 +3498,7 @@
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G61" s="20" t="s">
         <v>119</v>
@@ -3526,7 +3535,7 @@
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G62" s="20" t="s">
         <v>119</v>
@@ -3565,7 +3574,7 @@
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G63" s="20" t="s">
         <v>119</v>
@@ -3604,7 +3613,7 @@
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G64" s="20" t="s">
         <v>119</v>
@@ -3643,7 +3652,7 @@
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G65" s="20" t="s">
         <v>119</v>
@@ -3682,7 +3691,7 @@
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>119</v>
@@ -3719,7 +3728,7 @@
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G67" s="20" t="s">
         <v>119</v>
@@ -3756,7 +3765,7 @@
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G68" s="20" t="s">
         <v>119</v>
@@ -3793,7 +3802,7 @@
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G69" s="20" t="s">
         <v>119</v>
@@ -3830,7 +3839,7 @@
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G70" s="20" t="s">
         <v>119</v>
@@ -3867,7 +3876,7 @@
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>119</v>
@@ -3904,7 +3913,7 @@
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G72" s="20" t="s">
         <v>119</v>
@@ -3941,7 +3950,7 @@
       </c>
       <c r="E73" s="20"/>
       <c r="F73" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G73" s="20" t="s">
         <v>119</v>
@@ -3973,7 +3982,7 @@
       <c r="C74" s="20"/>
       <c r="E74" s="20"/>
       <c r="F74" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G74" s="20" t="s">
         <v>119</v>
@@ -4004,7 +4013,7 @@
       <c r="C75" s="20"/>
       <c r="E75" s="20"/>
       <c r="F75" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G75" s="20" t="s">
         <v>119</v>
@@ -4035,7 +4044,7 @@
       <c r="C76" s="20"/>
       <c r="E76" s="20"/>
       <c r="F76" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G76" s="20" t="s">
         <v>119</v>
@@ -4067,13 +4076,13 @@
         <v>113</v>
       </c>
       <c r="D77" s="50" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E77" s="49" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G77" s="20" t="s">
         <v>119</v>
@@ -4102,19 +4111,19 @@
         <v>72</v>
       </c>
       <c r="B78" s="49" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C78" s="20" t="s">
         <v>113</v>
       </c>
       <c r="D78" s="50" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E78" s="49" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>119</v>
@@ -4143,19 +4152,19 @@
         <v>73</v>
       </c>
       <c r="B79" s="49" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C79" s="20" t="s">
         <v>113</v>
       </c>
       <c r="D79" s="50" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E79" s="49" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G79" s="20" t="s">
         <v>119</v>
@@ -4184,19 +4193,19 @@
         <v>74</v>
       </c>
       <c r="B80" s="49" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C80" s="20" t="s">
         <v>113</v>
       </c>
       <c r="D80" s="50" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E80" s="49" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G80" s="20" t="s">
         <v>119</v>
@@ -4231,7 +4240,7 @@
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G81" s="20" t="s">
         <v>119</v>
@@ -4266,7 +4275,7 @@
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G82" s="20" t="s">
         <v>119</v>
@@ -4301,7 +4310,7 @@
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G83" s="20" t="s">
         <v>119</v>
@@ -4336,7 +4345,7 @@
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G84" s="20" t="s">
         <v>119</v>
@@ -4371,7 +4380,7 @@
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>119</v>
@@ -4399,14 +4408,14 @@
         <v>80</v>
       </c>
       <c r="B86" s="49" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C86" s="20" t="s">
         <v>113</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G86" s="20" t="s">
         <v>119</v>
@@ -4434,14 +4443,14 @@
         <v>81</v>
       </c>
       <c r="B87" s="49" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C87" s="20" t="s">
         <v>113</v>
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G87" s="20" t="s">
         <v>119</v>
@@ -4469,14 +4478,14 @@
         <v>82</v>
       </c>
       <c r="B88" s="49" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C88" s="20" t="s">
         <v>113</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G88" s="20" t="s">
         <v>119</v>
@@ -4510,13 +4519,13 @@
         <v>113</v>
       </c>
       <c r="D89" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E89" s="49" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F89" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G89" s="20" t="s">
         <v>119</v>
@@ -4545,16 +4554,16 @@
         <v>84</v>
       </c>
       <c r="B90" s="49" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D90" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E90" s="49" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F90" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G90" s="20" t="s">
         <v>119</v>
@@ -4583,16 +4592,16 @@
         <v>85</v>
       </c>
       <c r="B91" s="49" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D91" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E91" s="49" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F91" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G91" s="20" t="s">
         <v>119</v>
@@ -4621,19 +4630,19 @@
         <v>86</v>
       </c>
       <c r="B92" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C92" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D92" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E92" s="51" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F92" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G92" s="20" t="s">
         <v>119</v>
@@ -4661,19 +4670,19 @@
         <v>87</v>
       </c>
       <c r="B93" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C93" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D93" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E93" s="51" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F93" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G93" s="20" t="s">
         <v>119</v>
@@ -4701,19 +4710,19 @@
         <v>88</v>
       </c>
       <c r="B94" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C94" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D94" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E94" s="51" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F94" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G94" s="20" t="s">
         <v>119</v>
@@ -4741,19 +4750,19 @@
         <v>89</v>
       </c>
       <c r="B95" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C95" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D95" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="E95" s="51" t="s">
         <v>195</v>
       </c>
-      <c r="E95" s="51" t="s">
-        <v>199</v>
-      </c>
       <c r="F95" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G95" s="20" t="s">
         <v>119</v>
@@ -4781,19 +4790,19 @@
         <v>90</v>
       </c>
       <c r="B96" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C96" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D96" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E96" s="51" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F96" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G96" s="20" t="s">
         <v>119</v>
@@ -4821,19 +4830,19 @@
         <v>91</v>
       </c>
       <c r="B97" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C97" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D97" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E97" s="51" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F97" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G97" s="20" t="s">
         <v>119</v>
@@ -4861,19 +4870,19 @@
         <v>92</v>
       </c>
       <c r="B98" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C98" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D98" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E98" s="51" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F98" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G98" s="20" t="s">
         <v>119</v>
@@ -4901,19 +4910,19 @@
         <v>93</v>
       </c>
       <c r="B99" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C99" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D99" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E99" s="51" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F99" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G99" s="20" t="s">
         <v>119</v>
@@ -4941,19 +4950,19 @@
         <v>94</v>
       </c>
       <c r="B100" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C100" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D100" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E100" s="51" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F100" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G100" s="20" t="s">
         <v>119</v>
@@ -4981,19 +4990,19 @@
         <v>95</v>
       </c>
       <c r="B101" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C101" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D101" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E101" s="51" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F101" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G101" s="20" t="s">
         <v>119</v>
@@ -5021,19 +5030,19 @@
         <v>96</v>
       </c>
       <c r="B102" s="49" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C102" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D102" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E102" s="51" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F102" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G102" s="20" t="s">
         <v>119</v>
@@ -5068,7 +5077,7 @@
       </c>
       <c r="E103" s="20"/>
       <c r="F103" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G103" s="20" t="s">
         <v>119</v>
@@ -5102,7 +5111,7 @@
       </c>
       <c r="E104" s="20"/>
       <c r="F104" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G104" s="20" t="s">
         <v>119</v>
@@ -5136,7 +5145,7 @@
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G105" s="20" t="s">
         <v>119</v>
@@ -5170,7 +5179,7 @@
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G106" s="20" t="s">
         <v>119</v>
@@ -5207,7 +5216,7 @@
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G107" s="20" t="s">
         <v>119</v>
@@ -5244,7 +5253,7 @@
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G108" s="20" t="s">
         <v>119</v>
@@ -5281,7 +5290,7 @@
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G109" s="20" t="s">
         <v>119</v>
@@ -5318,7 +5327,7 @@
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G110" s="20" t="s">
         <v>119</v>
@@ -5355,7 +5364,7 @@
       </c>
       <c r="E111" s="20"/>
       <c r="F111" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G111" s="20" t="s">
         <v>119</v>
@@ -5392,7 +5401,7 @@
       </c>
       <c r="E112" s="20"/>
       <c r="F112" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G112" s="20" t="s">
         <v>119</v>
@@ -5429,7 +5438,7 @@
       </c>
       <c r="E113" s="20"/>
       <c r="F113" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G113" s="20" t="s">
         <v>119</v>
@@ -5466,7 +5475,7 @@
       </c>
       <c r="E114" s="20"/>
       <c r="F114" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G114" s="20" t="s">
         <v>119</v>
@@ -5503,7 +5512,7 @@
       </c>
       <c r="E115" s="20"/>
       <c r="F115" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G115" s="20" t="s">
         <v>119</v>
@@ -5540,7 +5549,7 @@
       </c>
       <c r="E116" s="20"/>
       <c r="F116" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G116" s="20" t="s">
         <v>119</v>
@@ -5577,7 +5586,7 @@
       </c>
       <c r="E117" s="20"/>
       <c r="F117" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G117" s="20" t="s">
         <v>119</v>
@@ -5614,7 +5623,7 @@
       </c>
       <c r="E118" s="20"/>
       <c r="F118" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G118" s="20" t="s">
         <v>119</v>
@@ -5651,7 +5660,7 @@
       </c>
       <c r="E119" s="20"/>
       <c r="F119" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G119" s="20" t="s">
         <v>119</v>
@@ -5684,13 +5693,13 @@
         <v>113</v>
       </c>
       <c r="D120" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E120" s="49" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F120" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G120" s="20" t="s">
         <v>119</v>
@@ -5725,13 +5734,13 @@
         <v>113</v>
       </c>
       <c r="D121" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E121" s="49" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F121" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G121" s="20" t="s">
         <v>119</v>
@@ -5766,13 +5775,13 @@
         <v>113</v>
       </c>
       <c r="D122" s="50" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E122" s="49" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F122" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G122" s="20" t="s">
         <v>119</v>
@@ -5800,8 +5809,8 @@
       <c r="A123" s="3">
         <v>121</v>
       </c>
-      <c r="B123" s="31" t="s">
-        <v>173</v>
+      <c r="B123" s="49" t="s">
+        <v>215</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>113</v>
@@ -5809,22 +5818,27 @@
       <c r="D123" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E123" s="20"/>
+      <c r="E123" s="49" t="s">
+        <v>221</v>
+      </c>
       <c r="F123" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G123" s="20" t="s">
         <v>119</v>
       </c>
       <c r="H123" s="22"/>
       <c r="I123" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J123" s="19">
         <f>340*9807000</f>
         <v>3334380000</v>
       </c>
-      <c r="K123" s="19"/>
+      <c r="K123" s="19">
+        <f>3*9807000</f>
+        <v>29421000</v>
+      </c>
       <c r="L123" s="20" t="s">
         <v>47</v>
       </c>
@@ -5839,28 +5853,36 @@
       <c r="A124" s="3">
         <v>122</v>
       </c>
-      <c r="B124" s="31" t="s">
-        <v>174</v>
+      <c r="B124" s="49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C124" s="50" t="s">
+        <v>113</v>
       </c>
       <c r="D124" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E124" s="20"/>
+      <c r="E124" s="49" t="s">
+        <v>221</v>
+      </c>
       <c r="F124" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G124" s="20" t="s">
         <v>119</v>
       </c>
       <c r="H124" s="22"/>
       <c r="I124" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J124" s="19">
         <f>357*9807000</f>
         <v>3501099000</v>
       </c>
-      <c r="K124" s="19"/>
+      <c r="K124" s="19">
+        <f>3*9807000</f>
+        <v>29421000</v>
+      </c>
       <c r="L124" s="20" t="s">
         <v>47</v>
       </c>
@@ -5875,28 +5897,36 @@
       <c r="A125" s="3">
         <v>123</v>
       </c>
-      <c r="B125" s="31" t="s">
-        <v>175</v>
+      <c r="B125" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="C125" s="50" t="s">
+        <v>219</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E125" s="20"/>
+      <c r="E125" s="49" t="s">
+        <v>221</v>
+      </c>
       <c r="F125" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G125" s="20" t="s">
         <v>119</v>
       </c>
       <c r="H125" s="22"/>
       <c r="I125" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J125" s="19">
         <f>457*9807000</f>
         <v>4481799000</v>
       </c>
-      <c r="K125" s="19"/>
+      <c r="K125" s="19">
+        <f>13*9807000</f>
+        <v>127491000</v>
+      </c>
       <c r="L125" s="20" t="s">
         <v>47</v>
       </c>
@@ -5911,28 +5941,36 @@
       <c r="A126" s="3">
         <v>124</v>
       </c>
-      <c r="B126" s="31" t="s">
-        <v>176</v>
+      <c r="B126" s="49" t="s">
+        <v>218</v>
+      </c>
+      <c r="C126" s="50" t="s">
+        <v>220</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E126" s="20"/>
+      <c r="E126" s="49" t="s">
+        <v>221</v>
+      </c>
       <c r="F126" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G126" s="20" t="s">
         <v>119</v>
       </c>
       <c r="H126" s="22"/>
       <c r="I126" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J126" s="19">
         <f>414*9807000</f>
         <v>4060098000</v>
       </c>
-      <c r="K126" s="19"/>
+      <c r="K126" s="19">
+        <f>8*9807000</f>
+        <v>78456000</v>
+      </c>
       <c r="L126" s="20" t="s">
         <v>47</v>
       </c>
@@ -5955,7 +5993,7 @@
       </c>
       <c r="E127" s="20"/>
       <c r="F127" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G127" s="20" t="s">
         <v>119</v>
@@ -5990,7 +6028,7 @@
       </c>
       <c r="E128" s="20"/>
       <c r="F128" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G128" s="20" t="s">
         <v>119</v>
@@ -6025,7 +6063,7 @@
       </c>
       <c r="E129" s="20"/>
       <c r="F129" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G129" s="20" t="s">
         <v>119</v>
@@ -6060,7 +6098,7 @@
       </c>
       <c r="E130" s="20"/>
       <c r="F130" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G130" s="20" t="s">
         <v>119</v>
@@ -6095,7 +6133,7 @@
       </c>
       <c r="E131" s="20"/>
       <c r="F131" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G131" s="20" t="s">
         <v>119</v>
@@ -6130,7 +6168,7 @@
       </c>
       <c r="E132" s="20"/>
       <c r="F132" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G132" s="20" t="s">
         <v>119</v>
@@ -6165,7 +6203,7 @@
       </c>
       <c r="E133" s="20"/>
       <c r="F133" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G133" s="20" t="s">
         <v>119</v>
@@ -6200,7 +6238,7 @@
       </c>
       <c r="E134" s="20"/>
       <c r="F134" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G134" s="20" t="s">
         <v>119</v>
@@ -6232,7 +6270,7 @@
       </c>
       <c r="E135" s="20"/>
       <c r="F135" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G135" s="20" t="s">
         <v>119</v>
@@ -6264,7 +6302,7 @@
       </c>
       <c r="E136" s="20"/>
       <c r="F136" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G136" s="20" t="s">
         <v>119</v>
@@ -6290,19 +6328,19 @@
         <v>135</v>
       </c>
       <c r="B137" s="31" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C137" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D137" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E137" s="51" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F137" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G137" s="20" t="s">
         <v>119</v>
@@ -6331,19 +6369,19 @@
         <v>136</v>
       </c>
       <c r="B138" s="31" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C138" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D138" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E138" s="51" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F138" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G138" s="20" t="s">
         <v>119</v>
@@ -6372,19 +6410,19 @@
         <v>137</v>
       </c>
       <c r="B139" s="31" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C139" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D139" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E139" s="51" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F139" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G139" s="20" t="s">
         <v>119</v>
@@ -6413,19 +6451,19 @@
         <v>138</v>
       </c>
       <c r="B140" s="31" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C140" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D140" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E140" s="51" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F140" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G140" s="20" t="s">
         <v>119</v>
@@ -6454,19 +6492,19 @@
         <v>139</v>
       </c>
       <c r="B141" s="31" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C141" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D141" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E141" s="51" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F141" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G141" s="20" t="s">
         <v>119</v>
@@ -6495,19 +6533,19 @@
         <v>140</v>
       </c>
       <c r="B142" s="31" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C142" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D142" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E142" s="51" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F142" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G142" s="20" t="s">
         <v>119</v>
@@ -6536,19 +6574,19 @@
         <v>141</v>
       </c>
       <c r="B143" s="31" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C143" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D143" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E143" s="51" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F143" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G143" s="20" t="s">
         <v>119</v>
@@ -6577,19 +6615,19 @@
         <v>142</v>
       </c>
       <c r="B144" s="31" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C144" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D144" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E144" s="51" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F144" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G144" s="20" t="s">
         <v>119</v>
@@ -6625,7 +6663,7 @@
       </c>
       <c r="E145" s="20"/>
       <c r="F145" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G145" s="20" t="s">
         <v>119</v>
@@ -6661,7 +6699,7 @@
       </c>
       <c r="E146" s="20"/>
       <c r="F146" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G146" s="20" t="s">
         <v>119</v>
@@ -6693,11 +6731,11 @@
         <v>107</v>
       </c>
       <c r="D147" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E147" s="20"/>
       <c r="F147" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G147" s="20" t="s">
         <v>119</v>
@@ -6729,11 +6767,11 @@
         <v>107</v>
       </c>
       <c r="D148" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E148" s="20"/>
       <c r="F148" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G148" s="20" t="s">
         <v>119</v>
@@ -6769,7 +6807,7 @@
       </c>
       <c r="E149" s="20"/>
       <c r="F149" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G149" s="20" t="s">
         <v>119</v>
@@ -6803,7 +6841,7 @@
       </c>
       <c r="E150" s="20"/>
       <c r="F150" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G150" s="20" t="s">
         <v>119</v>
@@ -6835,11 +6873,11 @@
         <v>108</v>
       </c>
       <c r="D151" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E151" s="20"/>
       <c r="F151" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G151" s="20" t="s">
         <v>119</v>
@@ -6871,11 +6909,11 @@
         <v>108</v>
       </c>
       <c r="D152" s="36" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E152" s="20"/>
       <c r="F152" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G152" s="20" t="s">
         <v>119</v>
@@ -6911,7 +6949,7 @@
       </c>
       <c r="E153" s="20"/>
       <c r="F153" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G153" s="20" t="s">
         <v>119</v>
@@ -6945,7 +6983,7 @@
       </c>
       <c r="E154" s="20"/>
       <c r="F154" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G154" s="20" t="s">
         <v>119</v>
@@ -6979,7 +7017,7 @@
       </c>
       <c r="E155" s="20"/>
       <c r="F155" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G155" s="20" t="s">
         <v>119</v>
@@ -7013,7 +7051,7 @@
       </c>
       <c r="E156" s="20"/>
       <c r="F156" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G156" s="20" t="s">
         <v>119</v>
@@ -7047,7 +7085,7 @@
       </c>
       <c r="E157" s="20"/>
       <c r="F157" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G157" s="20" t="s">
         <v>119</v>
@@ -7074,7 +7112,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="31" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>113</v>
@@ -7084,7 +7122,7 @@
       </c>
       <c r="E158" s="20"/>
       <c r="F158" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G158" s="20" t="s">
         <v>119</v>
@@ -7111,17 +7149,17 @@
         <v>157</v>
       </c>
       <c r="B159" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C159" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="D159" s="36" t="s">
         <v>181</v>
-      </c>
-      <c r="C159" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="D159" s="36" t="s">
-        <v>185</v>
       </c>
       <c r="E159" s="20"/>
       <c r="F159" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G159" s="20" t="s">
         <v>119</v>
@@ -7150,19 +7188,19 @@
         <v>158</v>
       </c>
       <c r="B160" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C160" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="D160" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C160" s="36" t="s">
-        <v>186</v>
-      </c>
-      <c r="D160" s="36" t="s">
-        <v>185</v>
-      </c>
       <c r="E160" s="31" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F160" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G160" s="20" t="s">
         <v>119</v>
@@ -7191,19 +7229,19 @@
         <v>159</v>
       </c>
       <c r="B161" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C161" s="36" t="s">
+        <v>183</v>
+      </c>
+      <c r="D161" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C161" s="36" t="s">
-        <v>187</v>
-      </c>
-      <c r="D161" s="36" t="s">
-        <v>185</v>
-      </c>
       <c r="E161" s="31" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F161" s="31" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G161" s="20" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
- fixed incorrectly reported compositions (very), temperature, and processing from `110.1007/s11661-018-4472-z`
</commit_message>
<xml_diff>
--- a/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
+++ b/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FA52D7-3300-AC44-A05A-CBBB34998A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F71F456-39A2-C948-9A33-313A134BE05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="235">
   <si>
     <t>Name:</t>
   </si>
@@ -560,12 +560,6 @@
     <t>Ti67.30 Nb24.03 Ta3.53 Fe5.14</t>
   </si>
   <si>
-    <t>Co24.9 Cr24.9 Mo24.9 Nb24.9 Ti0.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BCC + BCC </t>
-  </si>
-  <si>
     <t>Marcia Ahn</t>
   </si>
   <si>
@@ -575,15 +569,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>BCC + BCC + ?</t>
-  </si>
-  <si>
-    <t>BCC + CC + ?</t>
-  </si>
-  <si>
-    <t>? is precipitate</t>
-  </si>
-  <si>
     <t>hardness</t>
   </si>
   <si>
@@ -744,6 +729,30 @@
   </si>
   <si>
     <t>HT3 was homogenized at 1673K for 24h under vacuum and oil quenched; second annealing at 1073K for 24h under vacuum and oil quenched</t>
+  </si>
+  <si>
+    <t>CoCrNbMoTi0.4</t>
+  </si>
+  <si>
+    <t>AAM+A</t>
+  </si>
+  <si>
+    <t>annealed for 20h in vacuum at 1073K</t>
+  </si>
+  <si>
+    <t>annealed for 20h in vacuum at 1273K</t>
+  </si>
+  <si>
+    <t>500g vickers for 15s</t>
+  </si>
+  <si>
+    <t>BCC+BCC</t>
+  </si>
+  <si>
+    <t>BCC+BCC+laves</t>
+  </si>
+  <si>
+    <t>annealed for 20h in vacuum at 1473K; strong presence of laves phase</t>
   </si>
 </sst>
 </file>
@@ -926,7 +935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1036,6 +1045,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1324,8 +1336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G166" sqref="G166"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I169" sqref="I169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1359,14 +1371,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D2" s="44" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="44"/>
       <c r="F2" s="42" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G2" s="43"/>
       <c r="H2" s="43"/>
@@ -1383,7 +1395,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D3" s="44"/>
       <c r="E3" s="44"/>
@@ -1635,7 +1647,7 @@
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>114</v>
@@ -1675,7 +1687,7 @@
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>114</v>
@@ -1715,7 +1727,7 @@
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>114</v>
@@ -1755,7 +1767,7 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>114</v>
@@ -1795,7 +1807,7 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>114</v>
@@ -1835,7 +1847,7 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>114</v>
@@ -1875,7 +1887,7 @@
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>114</v>
@@ -1915,7 +1927,7 @@
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>114</v>
@@ -1954,7 +1966,7 @@
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>114</v>
@@ -1993,7 +2005,7 @@
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>114</v>
@@ -2032,7 +2044,7 @@
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>114</v>
@@ -2071,7 +2083,7 @@
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>114</v>
@@ -2110,7 +2122,7 @@
       </c>
       <c r="E22" s="20"/>
       <c r="F22" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>114</v>
@@ -2149,7 +2161,7 @@
       </c>
       <c r="E23" s="20"/>
       <c r="F23" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>114</v>
@@ -2188,7 +2200,7 @@
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>114</v>
@@ -2227,7 +2239,7 @@
       </c>
       <c r="E25" s="20"/>
       <c r="F25" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>114</v>
@@ -2266,7 +2278,7 @@
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>114</v>
@@ -2305,7 +2317,7 @@
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>114</v>
@@ -2344,7 +2356,7 @@
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>114</v>
@@ -2383,7 +2395,7 @@
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>114</v>
@@ -2422,7 +2434,7 @@
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>114</v>
@@ -2461,7 +2473,7 @@
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>114</v>
@@ -2500,7 +2512,7 @@
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>114</v>
@@ -2539,7 +2551,7 @@
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>114</v>
@@ -2578,7 +2590,7 @@
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>114</v>
@@ -2617,7 +2629,7 @@
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>114</v>
@@ -2653,7 +2665,7 @@
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>114</v>
@@ -2689,7 +2701,7 @@
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>114</v>
@@ -2725,7 +2737,7 @@
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>114</v>
@@ -2760,7 +2772,7 @@
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>114</v>
@@ -2795,7 +2807,7 @@
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>114</v>
@@ -2830,7 +2842,7 @@
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>114</v>
@@ -2864,7 +2876,7 @@
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>114</v>
@@ -2900,7 +2912,7 @@
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>114</v>
@@ -2936,7 +2948,7 @@
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>114</v>
@@ -2972,7 +2984,7 @@
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>114</v>
@@ -3008,7 +3020,7 @@
       </c>
       <c r="E46" s="20"/>
       <c r="F46" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>114</v>
@@ -3044,7 +3056,7 @@
       </c>
       <c r="E47" s="20"/>
       <c r="F47" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>114</v>
@@ -3080,7 +3092,7 @@
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>114</v>
@@ -3116,7 +3128,7 @@
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>114</v>
@@ -3152,7 +3164,7 @@
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>114</v>
@@ -3188,7 +3200,7 @@
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>114</v>
@@ -3221,7 +3233,7 @@
       <c r="C52" s="20"/>
       <c r="E52" s="20"/>
       <c r="F52" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>114</v>
@@ -3254,7 +3266,7 @@
       <c r="C53" s="20"/>
       <c r="E53" s="20"/>
       <c r="F53" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>114</v>
@@ -3287,7 +3299,7 @@
       <c r="C54" s="20"/>
       <c r="E54" s="20"/>
       <c r="F54" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>114</v>
@@ -3320,7 +3332,7 @@
       <c r="C55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>114</v>
@@ -3353,7 +3365,7 @@
       <c r="C56" s="20"/>
       <c r="E56" s="20"/>
       <c r="F56" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G56" s="20" t="s">
         <v>114</v>
@@ -3386,7 +3398,7 @@
       <c r="C57" s="20"/>
       <c r="E57" s="20"/>
       <c r="F57" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G57" s="20" t="s">
         <v>114</v>
@@ -3422,7 +3434,7 @@
       </c>
       <c r="E58" s="20"/>
       <c r="F58" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>114</v>
@@ -3457,7 +3469,7 @@
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>114</v>
@@ -3492,7 +3504,7 @@
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G60" s="20" t="s">
         <v>114</v>
@@ -3527,7 +3539,7 @@
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G61" s="20" t="s">
         <v>114</v>
@@ -3564,7 +3576,7 @@
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G62" s="20" t="s">
         <v>114</v>
@@ -3603,7 +3615,7 @@
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G63" s="20" t="s">
         <v>114</v>
@@ -3642,7 +3654,7 @@
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G64" s="20" t="s">
         <v>114</v>
@@ -3681,7 +3693,7 @@
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G65" s="20" t="s">
         <v>114</v>
@@ -3720,7 +3732,7 @@
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>114</v>
@@ -3757,7 +3769,7 @@
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G67" s="20" t="s">
         <v>114</v>
@@ -3794,7 +3806,7 @@
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G68" s="20" t="s">
         <v>114</v>
@@ -3831,7 +3843,7 @@
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G69" s="20" t="s">
         <v>114</v>
@@ -3868,7 +3880,7 @@
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G70" s="20" t="s">
         <v>114</v>
@@ -3905,7 +3917,7 @@
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>114</v>
@@ -3942,7 +3954,7 @@
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G72" s="20" t="s">
         <v>114</v>
@@ -3979,7 +3991,7 @@
       </c>
       <c r="E73" s="20"/>
       <c r="F73" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G73" s="20" t="s">
         <v>114</v>
@@ -4011,7 +4023,7 @@
       <c r="C74" s="20"/>
       <c r="E74" s="20"/>
       <c r="F74" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G74" s="20" t="s">
         <v>114</v>
@@ -4042,7 +4054,7 @@
       <c r="C75" s="20"/>
       <c r="E75" s="20"/>
       <c r="F75" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G75" s="20" t="s">
         <v>114</v>
@@ -4073,7 +4085,7 @@
       <c r="C76" s="20"/>
       <c r="E76" s="20"/>
       <c r="F76" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G76" s="20" t="s">
         <v>114</v>
@@ -4105,13 +4117,13 @@
         <v>109</v>
       </c>
       <c r="D77" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E77" s="48" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G77" s="20" t="s">
         <v>114</v>
@@ -4140,19 +4152,19 @@
         <v>72</v>
       </c>
       <c r="B78" s="48" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C78" s="20" t="s">
         <v>109</v>
       </c>
       <c r="D78" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E78" s="48" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>114</v>
@@ -4181,19 +4193,19 @@
         <v>73</v>
       </c>
       <c r="B79" s="48" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C79" s="20" t="s">
         <v>109</v>
       </c>
       <c r="D79" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E79" s="48" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G79" s="20" t="s">
         <v>114</v>
@@ -4222,19 +4234,19 @@
         <v>74</v>
       </c>
       <c r="B80" s="48" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C80" s="20" t="s">
         <v>109</v>
       </c>
       <c r="D80" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E80" s="48" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G80" s="20" t="s">
         <v>114</v>
@@ -4269,7 +4281,7 @@
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G81" s="20" t="s">
         <v>114</v>
@@ -4304,7 +4316,7 @@
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G82" s="20" t="s">
         <v>114</v>
@@ -4339,7 +4351,7 @@
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G83" s="20" t="s">
         <v>114</v>
@@ -4374,7 +4386,7 @@
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G84" s="20" t="s">
         <v>114</v>
@@ -4409,7 +4421,7 @@
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>114</v>
@@ -4437,14 +4449,14 @@
         <v>80</v>
       </c>
       <c r="B86" s="48" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C86" s="20" t="s">
         <v>109</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G86" s="20" t="s">
         <v>114</v>
@@ -4472,14 +4484,14 @@
         <v>81</v>
       </c>
       <c r="B87" s="48" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C87" s="20" t="s">
         <v>109</v>
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G87" s="20" t="s">
         <v>114</v>
@@ -4507,14 +4519,14 @@
         <v>82</v>
       </c>
       <c r="B88" s="48" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C88" s="20" t="s">
         <v>109</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G88" s="20" t="s">
         <v>114</v>
@@ -4548,13 +4560,13 @@
         <v>109</v>
       </c>
       <c r="D89" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E89" s="48" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F89" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G89" s="20" t="s">
         <v>114</v>
@@ -4583,16 +4595,16 @@
         <v>84</v>
       </c>
       <c r="B90" s="48" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D90" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E90" s="48" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F90" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G90" s="20" t="s">
         <v>114</v>
@@ -4621,16 +4633,16 @@
         <v>85</v>
       </c>
       <c r="B91" s="48" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D91" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E91" s="48" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="F91" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G91" s="20" t="s">
         <v>114</v>
@@ -4659,19 +4671,19 @@
         <v>86</v>
       </c>
       <c r="B92" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C92" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D92" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E92" s="50" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F92" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G92" s="20" t="s">
         <v>114</v>
@@ -4699,19 +4711,19 @@
         <v>87</v>
       </c>
       <c r="B93" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C93" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D93" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E93" s="50" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F93" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G93" s="20" t="s">
         <v>114</v>
@@ -4739,19 +4751,19 @@
         <v>88</v>
       </c>
       <c r="B94" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C94" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D94" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E94" s="50" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F94" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G94" s="20" t="s">
         <v>114</v>
@@ -4779,19 +4791,19 @@
         <v>89</v>
       </c>
       <c r="B95" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C95" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D95" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E95" s="50" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F95" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G95" s="20" t="s">
         <v>114</v>
@@ -4819,19 +4831,19 @@
         <v>90</v>
       </c>
       <c r="B96" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C96" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D96" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="E96" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="E96" s="50" t="s">
-        <v>189</v>
-      </c>
       <c r="F96" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G96" s="20" t="s">
         <v>114</v>
@@ -4859,19 +4871,19 @@
         <v>91</v>
       </c>
       <c r="B97" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C97" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D97" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E97" s="50" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F97" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G97" s="20" t="s">
         <v>114</v>
@@ -4899,19 +4911,19 @@
         <v>92</v>
       </c>
       <c r="B98" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C98" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D98" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E98" s="50" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F98" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G98" s="20" t="s">
         <v>114</v>
@@ -4939,19 +4951,19 @@
         <v>93</v>
       </c>
       <c r="B99" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C99" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D99" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E99" s="50" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F99" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G99" s="20" t="s">
         <v>114</v>
@@ -4979,19 +4991,19 @@
         <v>94</v>
       </c>
       <c r="B100" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C100" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D100" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E100" s="50" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F100" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G100" s="20" t="s">
         <v>114</v>
@@ -5019,19 +5031,19 @@
         <v>95</v>
       </c>
       <c r="B101" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C101" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D101" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E101" s="50" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F101" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G101" s="20" t="s">
         <v>114</v>
@@ -5059,19 +5071,19 @@
         <v>96</v>
       </c>
       <c r="B102" s="48" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C102" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D102" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E102" s="50" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F102" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G102" s="20" t="s">
         <v>114</v>
@@ -5106,7 +5118,7 @@
       </c>
       <c r="E103" s="20"/>
       <c r="F103" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G103" s="20" t="s">
         <v>114</v>
@@ -5140,7 +5152,7 @@
       </c>
       <c r="E104" s="20"/>
       <c r="F104" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G104" s="20" t="s">
         <v>114</v>
@@ -5174,7 +5186,7 @@
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G105" s="20" t="s">
         <v>114</v>
@@ -5208,7 +5220,7 @@
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G106" s="20" t="s">
         <v>114</v>
@@ -5245,7 +5257,7 @@
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G107" s="20" t="s">
         <v>114</v>
@@ -5282,7 +5294,7 @@
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G108" s="20" t="s">
         <v>114</v>
@@ -5319,7 +5331,7 @@
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G109" s="20" t="s">
         <v>114</v>
@@ -5356,7 +5368,7 @@
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G110" s="20" t="s">
         <v>114</v>
@@ -5393,7 +5405,7 @@
       </c>
       <c r="E111" s="20"/>
       <c r="F111" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G111" s="20" t="s">
         <v>114</v>
@@ -5430,7 +5442,7 @@
       </c>
       <c r="E112" s="20"/>
       <c r="F112" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G112" s="20" t="s">
         <v>114</v>
@@ -5467,7 +5479,7 @@
       </c>
       <c r="E113" s="20"/>
       <c r="F113" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G113" s="20" t="s">
         <v>114</v>
@@ -5504,7 +5516,7 @@
       </c>
       <c r="E114" s="20"/>
       <c r="F114" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G114" s="20" t="s">
         <v>114</v>
@@ -5541,7 +5553,7 @@
       </c>
       <c r="E115" s="20"/>
       <c r="F115" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G115" s="20" t="s">
         <v>114</v>
@@ -5578,7 +5590,7 @@
       </c>
       <c r="E116" s="20"/>
       <c r="F116" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G116" s="20" t="s">
         <v>114</v>
@@ -5615,7 +5627,7 @@
       </c>
       <c r="E117" s="20"/>
       <c r="F117" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G117" s="20" t="s">
         <v>114</v>
@@ -5652,7 +5664,7 @@
       </c>
       <c r="E118" s="20"/>
       <c r="F118" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G118" s="20" t="s">
         <v>114</v>
@@ -5689,7 +5701,7 @@
       </c>
       <c r="E119" s="20"/>
       <c r="F119" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G119" s="20" t="s">
         <v>114</v>
@@ -5722,13 +5734,13 @@
         <v>109</v>
       </c>
       <c r="D120" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E120" s="48" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F120" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G120" s="20" t="s">
         <v>114</v>
@@ -5763,13 +5775,13 @@
         <v>109</v>
       </c>
       <c r="D121" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E121" s="48" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F121" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G121" s="20" t="s">
         <v>114</v>
@@ -5804,13 +5816,13 @@
         <v>109</v>
       </c>
       <c r="D122" s="49" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E122" s="48" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F122" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G122" s="20" t="s">
         <v>114</v>
@@ -5839,7 +5851,7 @@
         <v>121</v>
       </c>
       <c r="B123" s="48" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>109</v>
@@ -5848,10 +5860,10 @@
         <v>112</v>
       </c>
       <c r="E123" s="48" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F123" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G123" s="20" t="s">
         <v>114</v>
@@ -5883,7 +5895,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="48" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C124" s="49" t="s">
         <v>109</v>
@@ -5892,10 +5904,10 @@
         <v>112</v>
       </c>
       <c r="E124" s="48" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F124" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G124" s="20" t="s">
         <v>114</v>
@@ -5927,19 +5939,19 @@
         <v>123</v>
       </c>
       <c r="B125" s="48" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C125" s="49" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E125" s="48" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F125" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G125" s="20" t="s">
         <v>114</v>
@@ -5971,19 +5983,19 @@
         <v>124</v>
       </c>
       <c r="B126" s="48" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C126" s="49" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>112</v>
       </c>
       <c r="E126" s="48" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F126" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G126" s="20" t="s">
         <v>114</v>
@@ -6015,24 +6027,24 @@
         <v>125</v>
       </c>
       <c r="B127" s="48" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C127" s="49" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D127" s="49" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E127" s="20"/>
       <c r="F127" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G127" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H127" s="22"/>
       <c r="I127" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J127" s="19">
         <v>1569000000</v>
@@ -6056,24 +6068,24 @@
         <v>126</v>
       </c>
       <c r="B128" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="C128" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="D128" s="49" t="s">
         <v>216</v>
-      </c>
-      <c r="C128" s="49" t="s">
-        <v>219</v>
-      </c>
-      <c r="D128" s="49" t="s">
-        <v>221</v>
       </c>
       <c r="E128" s="20"/>
       <c r="F128" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G128" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H128" s="22"/>
       <c r="I128" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J128" s="19">
         <v>1667000000</v>
@@ -6097,24 +6109,24 @@
         <v>127</v>
       </c>
       <c r="B129" s="48" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C129" s="49" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D129" s="49" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E129" s="20"/>
       <c r="F129" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G129" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H129" s="22"/>
       <c r="I129" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J129" s="19">
         <v>5139000000</v>
@@ -6138,24 +6150,24 @@
         <v>128</v>
       </c>
       <c r="B130" s="48" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C130" s="49" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D130" s="49" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E130" s="20"/>
       <c r="F130" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G130" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H130" s="22"/>
       <c r="I130" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J130" s="19">
         <v>6375000000</v>
@@ -6179,26 +6191,26 @@
         <v>129</v>
       </c>
       <c r="B131" s="48" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C131" s="49" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D131" s="49" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E131" s="48" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F131" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G131" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H131" s="22"/>
       <c r="I131" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J131" s="19">
         <v>1314000000</v>
@@ -6222,26 +6234,26 @@
         <v>130</v>
       </c>
       <c r="B132" s="48" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C132" s="49" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D132" s="49" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E132" s="48" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F132" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G132" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H132" s="22"/>
       <c r="I132" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J132" s="19">
         <v>1324000000</v>
@@ -6265,26 +6277,26 @@
         <v>131</v>
       </c>
       <c r="B133" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="C133" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="D133" s="49" t="s">
         <v>217</v>
       </c>
-      <c r="C133" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="D133" s="49" t="s">
-        <v>222</v>
-      </c>
       <c r="E133" s="48" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F133" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G133" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H133" s="22"/>
       <c r="I133" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J133" s="19">
         <v>5757000000</v>
@@ -6308,26 +6320,26 @@
         <v>132</v>
       </c>
       <c r="B134" s="48" t="s">
+        <v>213</v>
+      </c>
+      <c r="C134" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="D134" s="49" t="s">
+        <v>217</v>
+      </c>
+      <c r="E134" s="48" t="s">
         <v>218</v>
       </c>
-      <c r="C134" s="49" t="s">
-        <v>220</v>
-      </c>
-      <c r="D134" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="E134" s="48" t="s">
-        <v>223</v>
-      </c>
       <c r="F134" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G134" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H134" s="22"/>
       <c r="I134" s="23">
-        <v>1673</v>
+        <v>298</v>
       </c>
       <c r="J134" s="19">
         <v>6237000000</v>
@@ -6355,7 +6367,7 @@
       </c>
       <c r="E135" s="20"/>
       <c r="F135" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G135" s="20" t="s">
         <v>114</v>
@@ -6387,7 +6399,7 @@
       </c>
       <c r="E136" s="20"/>
       <c r="F136" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G136" s="20" t="s">
         <v>114</v>
@@ -6419,13 +6431,13 @@
         <v>109</v>
       </c>
       <c r="D137" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E137" s="50" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F137" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G137" s="20" t="s">
         <v>114</v>
@@ -6460,13 +6472,13 @@
         <v>109</v>
       </c>
       <c r="D138" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E138" s="50" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F138" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G138" s="20" t="s">
         <v>114</v>
@@ -6501,13 +6513,13 @@
         <v>109</v>
       </c>
       <c r="D139" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E139" s="50" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F139" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G139" s="20" t="s">
         <v>114</v>
@@ -6542,13 +6554,13 @@
         <v>109</v>
       </c>
       <c r="D140" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E140" s="50" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F140" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G140" s="20" t="s">
         <v>114</v>
@@ -6583,13 +6595,13 @@
         <v>109</v>
       </c>
       <c r="D141" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E141" s="50" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F141" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G141" s="20" t="s">
         <v>114</v>
@@ -6624,13 +6636,13 @@
         <v>109</v>
       </c>
       <c r="D142" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E142" s="50" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F142" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G142" s="20" t="s">
         <v>114</v>
@@ -6665,13 +6677,13 @@
         <v>109</v>
       </c>
       <c r="D143" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E143" s="50" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F143" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G143" s="20" t="s">
         <v>114</v>
@@ -6706,13 +6718,13 @@
         <v>109</v>
       </c>
       <c r="D144" s="36" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E144" s="50" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F144" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G144" s="20" t="s">
         <v>114</v>
@@ -6741,16 +6753,16 @@
         <v>143</v>
       </c>
       <c r="B145" s="48" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C145" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D145" s="49" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F145" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G145" s="20" t="s">
         <v>114</v>
@@ -6779,19 +6791,19 @@
         <v>144</v>
       </c>
       <c r="B146" s="48" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C146" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D146" s="49" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E146" s="48" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F146" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G146" s="20" t="s">
         <v>114</v>
@@ -6820,19 +6832,19 @@
         <v>145</v>
       </c>
       <c r="B147" s="48" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C147" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D147" s="49" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E147" s="48" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F147" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G147" s="20" t="s">
         <v>114</v>
@@ -6861,19 +6873,19 @@
         <v>146</v>
       </c>
       <c r="B148" s="48" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C148" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D148" s="49" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E148" s="48" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F148" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G148" s="20" t="s">
         <v>114</v>
@@ -6902,16 +6914,16 @@
         <v>147</v>
       </c>
       <c r="B149" s="48" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C149" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D149" s="49" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F149" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G149" s="20" t="s">
         <v>114</v>
@@ -6940,19 +6952,19 @@
         <v>148</v>
       </c>
       <c r="B150" s="48" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C150" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D150" s="49" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E150" s="48" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F150" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G150" s="20" t="s">
         <v>114</v>
@@ -6981,19 +6993,19 @@
         <v>149</v>
       </c>
       <c r="B151" s="48" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C151" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D151" s="49" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E151" s="48" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F151" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G151" s="20" t="s">
         <v>114</v>
@@ -7022,19 +7034,19 @@
         <v>150</v>
       </c>
       <c r="B152" s="48" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C152" s="49" t="s">
         <v>109</v>
       </c>
       <c r="D152" s="49" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E152" s="48" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F152" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G152" s="20" t="s">
         <v>114</v>
@@ -7070,7 +7082,7 @@
       </c>
       <c r="E153" s="20"/>
       <c r="F153" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G153" s="20" t="s">
         <v>114</v>
@@ -7104,7 +7116,7 @@
       </c>
       <c r="E154" s="20"/>
       <c r="F154" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G154" s="20" t="s">
         <v>114</v>
@@ -7138,7 +7150,7 @@
       </c>
       <c r="E155" s="20"/>
       <c r="F155" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G155" s="20" t="s">
         <v>114</v>
@@ -7172,7 +7184,7 @@
       </c>
       <c r="E156" s="20"/>
       <c r="F156" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G156" s="20" t="s">
         <v>114</v>
@@ -7206,7 +7218,7 @@
       </c>
       <c r="E157" s="20"/>
       <c r="F157" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G157" s="20" t="s">
         <v>114</v>
@@ -7232,29 +7244,36 @@
       <c r="A158" s="3">
         <v>156</v>
       </c>
-      <c r="B158" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D158" s="3" t="s">
-        <v>111</v>
+      <c r="B158" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="C158" s="49" t="s">
+        <v>232</v>
+      </c>
+      <c r="D158" s="49" t="s">
+        <v>216</v>
       </c>
       <c r="E158" s="20"/>
       <c r="F158" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G158" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="H158" s="22"/>
-      <c r="I158" s="23"/>
+      <c r="H158" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="I158" s="23">
+        <v>298</v>
+      </c>
       <c r="J158" s="19">
         <f>829*9807000</f>
         <v>8130003000</v>
       </c>
-      <c r="K158" s="19"/>
+      <c r="K158" s="19">
+        <f>1*9807000</f>
+        <v>9807000</v>
+      </c>
       <c r="L158" s="20" t="s">
         <v>47</v>
       </c>
@@ -7269,31 +7288,38 @@
       <c r="A159" s="3">
         <v>157</v>
       </c>
-      <c r="B159" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="C159" s="36" t="s">
-        <v>171</v>
-      </c>
-      <c r="D159" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="E159" s="20"/>
+      <c r="B159" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="C159" s="49" t="s">
+        <v>233</v>
+      </c>
+      <c r="D159" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="E159" s="48" t="s">
+        <v>229</v>
+      </c>
       <c r="F159" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G159" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="H159" s="22"/>
+      <c r="H159" s="51" t="s">
+        <v>231</v>
+      </c>
       <c r="I159" s="23">
-        <v>1073</v>
+        <v>298</v>
       </c>
       <c r="J159" s="19">
         <f>920*9807000</f>
         <v>9022440000</v>
       </c>
-      <c r="K159" s="19"/>
+      <c r="K159" s="19">
+        <f>1*9807000</f>
+        <v>9807000</v>
+      </c>
       <c r="L159" s="20" t="s">
         <v>47</v>
       </c>
@@ -7308,33 +7334,38 @@
       <c r="A160" s="3">
         <v>158</v>
       </c>
-      <c r="B160" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="C160" s="36" t="s">
-        <v>175</v>
-      </c>
-      <c r="D160" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="E160" s="31" t="s">
-        <v>177</v>
+      <c r="B160" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="C160" s="49" t="s">
+        <v>233</v>
+      </c>
+      <c r="D160" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="E160" s="48" t="s">
+        <v>230</v>
       </c>
       <c r="F160" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G160" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="H160" s="22"/>
+      <c r="H160" s="51" t="s">
+        <v>231</v>
+      </c>
       <c r="I160" s="23">
-        <v>1273</v>
+        <v>298</v>
       </c>
       <c r="J160" s="19">
         <f>931*9807000</f>
         <v>9130317000</v>
       </c>
-      <c r="K160" s="19"/>
+      <c r="K160" s="19">
+        <f>2*9807000</f>
+        <v>19614000</v>
+      </c>
       <c r="L160" s="20" t="s">
         <v>47</v>
       </c>
@@ -7349,33 +7380,38 @@
       <c r="A161" s="3">
         <v>159</v>
       </c>
-      <c r="B161" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="C161" s="36" t="s">
-        <v>176</v>
-      </c>
-      <c r="D161" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="E161" s="31" t="s">
-        <v>177</v>
+      <c r="B161" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="C161" s="49" t="s">
+        <v>233</v>
+      </c>
+      <c r="D161" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="E161" s="48" t="s">
+        <v>234</v>
       </c>
       <c r="F161" s="31" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="G161" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="H161" s="22"/>
+      <c r="H161" s="51" t="s">
+        <v>231</v>
+      </c>
       <c r="I161" s="23">
-        <v>1473</v>
+        <v>298</v>
       </c>
       <c r="J161" s="19">
         <f>960*9807000</f>
         <v>9414720000</v>
       </c>
-      <c r="K161" s="19"/>
+      <c r="K161" s="19">
+        <f>2*9807000</f>
+        <v>19614000</v>
+      </c>
       <c r="L161" s="20" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
- fixed incorrectly reported temperature and processing from `10.1016/j.ijrmhm.2016.04.020`
</commit_message>
<xml_diff>
--- a/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
+++ b/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F71F456-39A2-C948-9A33-313A134BE05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B39DE38-F023-2340-BFEF-F6C94C061B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="238">
   <si>
     <t>Name:</t>
   </si>
@@ -753,6 +753,15 @@
   </si>
   <si>
     <t>annealed for 20h in vacuum at 1473K; strong presence of laves phase</t>
+  </si>
+  <si>
+    <t>sintered at 1420*C for 30min under 40MPa</t>
+  </si>
+  <si>
+    <t>BCC+Mo2C</t>
+  </si>
+  <si>
+    <t>BCC+Mo2C+Mo2B</t>
   </si>
 </sst>
 </file>
@@ -1336,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I169" sqref="I169"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -3263,8 +3272,15 @@
       <c r="B53" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C53" s="20"/>
-      <c r="E53" s="20"/>
+      <c r="C53" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="E53" s="48" t="s">
+        <v>235</v>
+      </c>
       <c r="F53" s="31" t="s">
         <v>173</v>
       </c>
@@ -3273,12 +3289,14 @@
       </c>
       <c r="H53" s="22"/>
       <c r="I53" s="23">
-        <v>1273</v>
+        <v>298</v>
       </c>
       <c r="J53" s="19">
         <v>1900000000</v>
       </c>
-      <c r="K53" s="19"/>
+      <c r="K53" s="19">
+        <v>30000000</v>
+      </c>
       <c r="L53" s="20" t="s">
         <v>47</v>
       </c>
@@ -3296,8 +3314,15 @@
       <c r="B54" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="C54" s="20"/>
-      <c r="E54" s="20"/>
+      <c r="C54" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="E54" s="48" t="s">
+        <v>235</v>
+      </c>
       <c r="F54" s="31" t="s">
         <v>173</v>
       </c>
@@ -3306,12 +3331,14 @@
       </c>
       <c r="H54" s="22"/>
       <c r="I54" s="23">
-        <v>1273</v>
+        <v>298</v>
       </c>
       <c r="J54" s="19">
         <v>2100000000</v>
       </c>
-      <c r="K54" s="19"/>
+      <c r="K54" s="19">
+        <v>20000000</v>
+      </c>
       <c r="L54" s="20" t="s">
         <v>47</v>
       </c>
@@ -3329,8 +3356,15 @@
       <c r="B55" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="C55" s="20"/>
-      <c r="E55" s="20"/>
+      <c r="C55" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="D55" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="E55" s="48" t="s">
+        <v>235</v>
+      </c>
       <c r="F55" s="31" t="s">
         <v>173</v>
       </c>
@@ -3339,12 +3373,14 @@
       </c>
       <c r="H55" s="22"/>
       <c r="I55" s="23">
-        <v>1273</v>
+        <v>298</v>
       </c>
       <c r="J55" s="19">
         <v>3400000000</v>
       </c>
-      <c r="K55" s="19"/>
+      <c r="K55" s="19">
+        <v>40000000</v>
+      </c>
       <c r="L55" s="20" t="s">
         <v>47</v>
       </c>
@@ -3362,8 +3398,15 @@
       <c r="B56" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="C56" s="20"/>
-      <c r="E56" s="20"/>
+      <c r="C56" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="D56" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="E56" s="48" t="s">
+        <v>235</v>
+      </c>
       <c r="F56" s="31" t="s">
         <v>173</v>
       </c>
@@ -3372,19 +3415,21 @@
       </c>
       <c r="H56" s="22"/>
       <c r="I56" s="23">
-        <v>1273</v>
+        <v>298</v>
       </c>
       <c r="J56" s="19">
         <v>5200000000</v>
       </c>
-      <c r="K56" s="19"/>
+      <c r="K56" s="19">
+        <v>20000000</v>
+      </c>
       <c r="L56" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M56" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="N56" s="3" t="s">
+      <c r="N56" s="49" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3395,8 +3440,15 @@
       <c r="B57" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="C57" s="20"/>
-      <c r="E57" s="20"/>
+      <c r="C57" s="48" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="E57" s="48" t="s">
+        <v>235</v>
+      </c>
       <c r="F57" s="31" t="s">
         <v>173</v>
       </c>
@@ -3405,12 +3457,14 @@
       </c>
       <c r="H57" s="22"/>
       <c r="I57" s="23">
-        <v>1273</v>
+        <v>298</v>
       </c>
       <c r="J57" s="19">
         <v>7800000000</v>
       </c>
-      <c r="K57" s="19"/>
+      <c r="K57" s="19">
+        <v>10000000</v>
+      </c>
       <c r="L57" s="20" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
- removed data from `10.3390/ma11010069` as the paper did not support it
</commit_message>
<xml_diff>
--- a/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
+++ b/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1369CAA-65E9-AE41-8A4B-369CAB8F861A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55D0ECB-2AA6-234E-B289-CEFA9D346814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9300" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="236">
   <si>
     <t>Name:</t>
   </si>
@@ -354,9 +354,6 @@
     <t>HIP + A</t>
   </si>
   <si>
-    <t>beta</t>
-  </si>
-  <si>
     <t xml:space="preserve">EXP </t>
   </si>
   <si>
@@ -427,9 +424,6 @@
   </si>
   <si>
     <t>T4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.3390/ma11010069 </t>
   </si>
   <si>
     <t>10.3390/met9010076</t>
@@ -483,9 +477,6 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2013.12.210</t>
-  </si>
-  <si>
-    <t>Nb40.7 Ti12.8 Mo4.7 W1.3 Hf1.5 Cr2.7 Si20.8 Ge5.9 Al4.6 Sn5</t>
   </si>
   <si>
     <t>Mo98.79 Ti1.0 Zr0.08 C0.13</t>
@@ -1344,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T407"/>
+  <dimension ref="A1:T406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1381,14 +1372,14 @@
         <v>0</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D2" s="42" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="42"/>
       <c r="F2" s="40" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
@@ -1405,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D3" s="42"/>
       <c r="E3" s="42"/>
@@ -1466,7 +1457,7 @@
         <v>30</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="N5" s="39" t="s">
         <v>46</v>
@@ -1654,10 +1645,10 @@
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="23">
@@ -1672,10 +1663,10 @@
         <v>47</v>
       </c>
       <c r="M10" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="N10" s="25" t="s">
         <v>108</v>
-      </c>
-      <c r="N10" s="25" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1690,10 +1681,10 @@
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="23">
@@ -1708,10 +1699,10 @@
         <v>47</v>
       </c>
       <c r="M11" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" s="25" t="s">
         <v>108</v>
-      </c>
-      <c r="N11" s="25" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:20">
@@ -1726,10 +1717,10 @@
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="23">
@@ -1743,10 +1734,10 @@
         <v>47</v>
       </c>
       <c r="M12" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="N12" s="25" t="s">
         <v>108</v>
-      </c>
-      <c r="N12" s="25" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1761,10 +1752,10 @@
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="23">
@@ -1778,10 +1769,10 @@
         <v>47</v>
       </c>
       <c r="M13" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" s="25" t="s">
         <v>108</v>
-      </c>
-      <c r="N13" s="25" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1796,10 +1787,10 @@
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="23">
@@ -1813,10 +1804,10 @@
         <v>47</v>
       </c>
       <c r="M14" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="N14" s="25" t="s">
         <v>108</v>
-      </c>
-      <c r="N14" s="25" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -1831,10 +1822,10 @@
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="23">
@@ -1849,7 +1840,7 @@
       </c>
       <c r="M15" s="20"/>
       <c r="N15" s="25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -1857,22 +1848,22 @@
         <v>37</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C16" s="46" t="s">
         <v>103</v>
       </c>
       <c r="D16" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="F16" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="F16" s="46" t="s">
-        <v>238</v>
-      </c>
       <c r="G16" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="23">
@@ -1886,10 +1877,10 @@
         <v>47</v>
       </c>
       <c r="M16" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N16" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1900,19 +1891,19 @@
         <v>66</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D17" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="F17" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="E17" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="F17" s="46" t="s">
-        <v>238</v>
-      </c>
       <c r="G17" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="23">
@@ -1926,10 +1917,10 @@
         <v>47</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N17" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1937,20 +1928,20 @@
         <v>39</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="F18" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="E18" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="F18" s="46" t="s">
-        <v>238</v>
-      </c>
       <c r="G18" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="23">
@@ -1964,10 +1955,10 @@
         <v>47</v>
       </c>
       <c r="M18" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N18" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1975,20 +1966,20 @@
         <v>40</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="F19" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="E19" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="F19" s="46" t="s">
-        <v>238</v>
-      </c>
       <c r="G19" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="23">
@@ -2002,10 +1993,10 @@
         <v>47</v>
       </c>
       <c r="M19" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N19" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -2017,16 +2008,16 @@
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="F20" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="E20" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="F20" s="46" t="s">
-        <v>238</v>
-      </c>
       <c r="G20" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="23">
@@ -2040,10 +2031,10 @@
         <v>47</v>
       </c>
       <c r="M20" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N20" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -2055,16 +2046,16 @@
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="47" t="s">
+        <v>232</v>
+      </c>
+      <c r="E21" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="F21" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="E21" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="F21" s="46" t="s">
-        <v>238</v>
-      </c>
       <c r="G21" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H21" s="22"/>
       <c r="I21" s="23">
@@ -2078,10 +2069,10 @@
         <v>47</v>
       </c>
       <c r="M21" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N21" s="33" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -2094,10 +2085,10 @@
       <c r="C22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="23">
@@ -2111,10 +2102,10 @@
         <v>47</v>
       </c>
       <c r="M22" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N22" s="26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -2122,22 +2113,22 @@
         <v>44</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C23" s="46" t="s">
         <v>103</v>
       </c>
       <c r="D23" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F23" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="23">
@@ -2153,10 +2144,10 @@
         <v>47</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N23" s="25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -2164,22 +2155,22 @@
         <v>45</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C24" s="46" t="s">
         <v>103</v>
       </c>
       <c r="D24" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E24" s="46" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="23">
@@ -2195,10 +2186,10 @@
         <v>47</v>
       </c>
       <c r="M24" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N24" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -2206,22 +2197,22 @@
         <v>46</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D25" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="23">
@@ -2237,10 +2228,10 @@
         <v>47</v>
       </c>
       <c r="M25" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N25" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -2248,22 +2239,22 @@
         <v>47</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D26" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E26" s="46" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="23">
@@ -2279,10 +2270,10 @@
         <v>47</v>
       </c>
       <c r="M26" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N26" s="47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -2290,22 +2281,22 @@
         <v>48</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D27" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E27" s="46" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H27" s="22"/>
       <c r="I27" s="23">
@@ -2321,10 +2312,10 @@
         <v>47</v>
       </c>
       <c r="M27" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N27" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -2332,20 +2323,20 @@
         <v>49</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D28" s="47" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H28" s="22"/>
       <c r="I28" s="23">
@@ -2363,10 +2354,10 @@
         <v>47</v>
       </c>
       <c r="M28" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N28" s="25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -2374,20 +2365,20 @@
         <v>50</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D29" s="47" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="23">
@@ -2405,10 +2396,10 @@
         <v>47</v>
       </c>
       <c r="M29" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2416,20 +2407,20 @@
         <v>51</v>
       </c>
       <c r="B30" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="C30" s="46" t="s">
         <v>228</v>
       </c>
-      <c r="C30" s="46" t="s">
-        <v>231</v>
-      </c>
       <c r="D30" s="47" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="23">
@@ -2447,10 +2438,10 @@
         <v>47</v>
       </c>
       <c r="M30" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N30" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2458,20 +2449,20 @@
         <v>52</v>
       </c>
       <c r="B31" s="46" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="23">
@@ -2489,10 +2480,10 @@
         <v>47</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -2500,22 +2491,22 @@
         <v>53</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="23">
@@ -2533,10 +2524,10 @@
         <v>47</v>
       </c>
       <c r="M32" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2544,22 +2535,22 @@
         <v>54</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D33" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F33" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="23">
@@ -2577,10 +2568,10 @@
         <v>47</v>
       </c>
       <c r="M33" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N33" s="47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2588,22 +2579,22 @@
         <v>55</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D34" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E34" s="46" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H34" s="22"/>
       <c r="I34" s="23">
@@ -2621,10 +2612,10 @@
         <v>47</v>
       </c>
       <c r="M34" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2632,22 +2623,22 @@
         <v>56</v>
       </c>
       <c r="B35" s="46" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C35" s="46" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D35" s="47" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F35" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H35" s="22"/>
       <c r="I35" s="23">
@@ -2665,10 +2656,10 @@
         <v>47</v>
       </c>
       <c r="M35" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2686,10 +2677,10 @@
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H36" s="22"/>
       <c r="I36" s="23"/>
@@ -2702,10 +2693,10 @@
         <v>47</v>
       </c>
       <c r="M36" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N36" s="25" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2723,10 +2714,10 @@
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H37" s="22"/>
       <c r="I37" s="23"/>
@@ -2739,10 +2730,10 @@
         <v>47</v>
       </c>
       <c r="M37" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2760,10 +2751,10 @@
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H38" s="22"/>
       <c r="I38" s="23"/>
@@ -2776,10 +2767,10 @@
         <v>47</v>
       </c>
       <c r="M38" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2797,10 +2788,10 @@
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H39" s="22"/>
       <c r="I39" s="23"/>
@@ -2813,10 +2804,10 @@
         <v>47</v>
       </c>
       <c r="M39" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2834,10 +2825,10 @@
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H40" s="22"/>
       <c r="I40" s="23"/>
@@ -2850,10 +2841,10 @@
         <v>47</v>
       </c>
       <c r="M40" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N40" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2871,10 +2862,10 @@
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H41" s="22"/>
       <c r="I41" s="23"/>
@@ -2887,10 +2878,10 @@
         <v>47</v>
       </c>
       <c r="M41" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2908,10 +2899,10 @@
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H42" s="22"/>
       <c r="I42" s="23"/>
@@ -2924,10 +2915,10 @@
         <v>47</v>
       </c>
       <c r="M42" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N42" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2945,10 +2936,10 @@
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H43" s="22"/>
       <c r="I43" s="23"/>
@@ -2961,10 +2952,10 @@
         <v>47</v>
       </c>
       <c r="M43" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2978,16 +2969,16 @@
         <v>103</v>
       </c>
       <c r="D44" s="47" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F44" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G44" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H44" s="22"/>
       <c r="I44" s="23">
@@ -3002,10 +2993,10 @@
         <v>47</v>
       </c>
       <c r="M44" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="N44" s="25" t="s">
         <v>116</v>
-      </c>
-      <c r="N44" s="25" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -3013,22 +3004,22 @@
         <v>72</v>
       </c>
       <c r="B45" s="46" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D45" s="47" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F45" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G45" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H45" s="22"/>
       <c r="I45" s="23">
@@ -3043,10 +3034,10 @@
         <v>47</v>
       </c>
       <c r="M45" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="N45" s="25" t="s">
         <v>116</v>
-      </c>
-      <c r="N45" s="25" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -3054,22 +3045,22 @@
         <v>73</v>
       </c>
       <c r="B46" s="46" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D46" s="47" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F46" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H46" s="22"/>
       <c r="I46" s="23">
@@ -3084,10 +3075,10 @@
         <v>47</v>
       </c>
       <c r="M46" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="N46" s="25" t="s">
         <v>116</v>
-      </c>
-      <c r="N46" s="25" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -3095,22 +3086,22 @@
         <v>74</v>
       </c>
       <c r="B47" s="46" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>103</v>
       </c>
       <c r="D47" s="47" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E47" s="46" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F47" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G47" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H47" s="22"/>
       <c r="I47" s="23">
@@ -3124,10 +3115,10 @@
         <v>47</v>
       </c>
       <c r="M47" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="N47" s="25" t="s">
         <v>116</v>
-      </c>
-      <c r="N47" s="25" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -3142,10 +3133,10 @@
       </c>
       <c r="E48" s="20"/>
       <c r="F48" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G48" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H48" s="22"/>
       <c r="I48" s="23">
@@ -3159,10 +3150,10 @@
         <v>47</v>
       </c>
       <c r="M48" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N48" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="N48" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -3177,10 +3168,10 @@
       </c>
       <c r="E49" s="20"/>
       <c r="F49" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G49" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H49" s="22"/>
       <c r="I49" s="23">
@@ -3194,10 +3185,10 @@
         <v>47</v>
       </c>
       <c r="M49" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N49" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="N49" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -3212,10 +3203,10 @@
       </c>
       <c r="E50" s="20"/>
       <c r="F50" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H50" s="22"/>
       <c r="I50" s="23">
@@ -3229,10 +3220,10 @@
         <v>47</v>
       </c>
       <c r="M50" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N50" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="N50" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -3247,10 +3238,10 @@
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G51" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H51" s="22"/>
       <c r="I51" s="23">
@@ -3264,10 +3255,10 @@
         <v>47</v>
       </c>
       <c r="M51" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N51" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="N51" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -3282,10 +3273,10 @@
       </c>
       <c r="E52" s="20"/>
       <c r="F52" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G52" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H52" s="22"/>
       <c r="I52" s="23">
@@ -3299,10 +3290,10 @@
         <v>47</v>
       </c>
       <c r="M52" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N52" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="N52" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -3310,17 +3301,17 @@
         <v>80</v>
       </c>
       <c r="B53" s="46" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>103</v>
       </c>
       <c r="E53" s="20"/>
       <c r="F53" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G53" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H53" s="22"/>
       <c r="I53" s="23">
@@ -3334,10 +3325,10 @@
         <v>47</v>
       </c>
       <c r="M53" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N53" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="N53" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -3345,17 +3336,17 @@
         <v>81</v>
       </c>
       <c r="B54" s="46" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>103</v>
       </c>
       <c r="E54" s="20"/>
       <c r="F54" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G54" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H54" s="22"/>
       <c r="I54" s="23">
@@ -3369,10 +3360,10 @@
         <v>47</v>
       </c>
       <c r="M54" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N54" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="N54" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -3380,17 +3371,17 @@
         <v>82</v>
       </c>
       <c r="B55" s="46" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C55" s="20" t="s">
         <v>103</v>
       </c>
       <c r="E55" s="20"/>
       <c r="F55" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G55" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H55" s="22"/>
       <c r="I55" s="23">
@@ -3404,10 +3395,10 @@
         <v>47</v>
       </c>
       <c r="M55" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N55" s="25" t="s">
         <v>118</v>
-      </c>
-      <c r="N55" s="25" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -3421,16 +3412,16 @@
         <v>103</v>
       </c>
       <c r="D56" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E56" s="46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F56" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G56" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H56" s="22"/>
       <c r="I56" s="23">
@@ -3445,10 +3436,10 @@
         <v>47</v>
       </c>
       <c r="M56" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="N56" s="25" t="s">
         <v>120</v>
-      </c>
-      <c r="N56" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -3456,19 +3447,19 @@
         <v>84</v>
       </c>
       <c r="B57" s="46" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D57" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E57" s="46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F57" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G57" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H57" s="22"/>
       <c r="I57" s="23">
@@ -3483,10 +3474,10 @@
         <v>47</v>
       </c>
       <c r="M57" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="N57" s="25" t="s">
         <v>120</v>
-      </c>
-      <c r="N57" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -3494,19 +3485,19 @@
         <v>85</v>
       </c>
       <c r="B58" s="46" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D58" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E58" s="46" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F58" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G58" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H58" s="22"/>
       <c r="I58" s="23">
@@ -3521,10 +3512,10 @@
         <v>47</v>
       </c>
       <c r="M58" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="N58" s="25" t="s">
         <v>120</v>
-      </c>
-      <c r="N58" s="25" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3532,22 +3523,22 @@
         <v>86</v>
       </c>
       <c r="B59" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C59" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D59" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E59" s="48" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F59" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H59" s="22"/>
       <c r="I59" s="3">
@@ -3561,10 +3552,10 @@
         <v>47</v>
       </c>
       <c r="M59" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N59" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -3572,22 +3563,22 @@
         <v>87</v>
       </c>
       <c r="B60" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C60" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D60" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E60" s="48" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F60" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H60" s="22"/>
       <c r="I60" s="3">
@@ -3601,10 +3592,10 @@
         <v>47</v>
       </c>
       <c r="M60" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N60" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -3612,22 +3603,22 @@
         <v>88</v>
       </c>
       <c r="B61" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C61" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D61" s="47" t="s">
+        <v>162</v>
+      </c>
+      <c r="E61" s="48" t="s">
         <v>165</v>
       </c>
-      <c r="E61" s="48" t="s">
-        <v>168</v>
-      </c>
       <c r="F61" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H61" s="22"/>
       <c r="I61" s="3">
@@ -3641,10 +3632,10 @@
         <v>47</v>
       </c>
       <c r="M61" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N61" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -3652,22 +3643,22 @@
         <v>89</v>
       </c>
       <c r="B62" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C62" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D62" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E62" s="48" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F62" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H62" s="22"/>
       <c r="I62" s="3">
@@ -3681,10 +3672,10 @@
         <v>47</v>
       </c>
       <c r="M62" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N62" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -3692,22 +3683,22 @@
         <v>90</v>
       </c>
       <c r="B63" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C63" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E63" s="48" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F63" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H63" s="22"/>
       <c r="I63" s="3">
@@ -3721,10 +3712,10 @@
         <v>47</v>
       </c>
       <c r="M63" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N63" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -3732,22 +3723,22 @@
         <v>91</v>
       </c>
       <c r="B64" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C64" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D64" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E64" s="48" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F64" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H64" s="22"/>
       <c r="I64" s="3">
@@ -3761,10 +3752,10 @@
         <v>47</v>
       </c>
       <c r="M64" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N64" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:14">
@@ -3772,22 +3763,22 @@
         <v>92</v>
       </c>
       <c r="B65" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C65" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D65" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E65" s="48" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F65" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G65" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H65" s="22"/>
       <c r="I65" s="3">
@@ -3801,10 +3792,10 @@
         <v>47</v>
       </c>
       <c r="M65" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N65" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -3812,22 +3803,22 @@
         <v>93</v>
       </c>
       <c r="B66" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C66" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D66" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E66" s="48" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F66" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G66" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H66" s="22"/>
       <c r="I66" s="3">
@@ -3841,10 +3832,10 @@
         <v>47</v>
       </c>
       <c r="M66" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N66" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -3852,22 +3843,22 @@
         <v>94</v>
       </c>
       <c r="B67" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C67" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D67" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E67" s="48" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F67" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G67" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H67" s="22"/>
       <c r="I67" s="3">
@@ -3881,10 +3872,10 @@
         <v>47</v>
       </c>
       <c r="M67" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N67" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:14">
@@ -3892,22 +3883,22 @@
         <v>95</v>
       </c>
       <c r="B68" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C68" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D68" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E68" s="48" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F68" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G68" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H68" s="22"/>
       <c r="I68" s="3">
@@ -3921,10 +3912,10 @@
         <v>47</v>
       </c>
       <c r="M68" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N68" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -3932,22 +3923,22 @@
         <v>96</v>
       </c>
       <c r="B69" s="46" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C69" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D69" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E69" s="48" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F69" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G69" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H69" s="22"/>
       <c r="I69" s="3">
@@ -3961,10 +3952,10 @@
         <v>47</v>
       </c>
       <c r="M69" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N69" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:14">
@@ -3979,10 +3970,10 @@
       </c>
       <c r="E70" s="20"/>
       <c r="F70" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G70" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H70" s="22"/>
       <c r="I70" s="23"/>
@@ -3995,10 +3986,10 @@
         <v>47</v>
       </c>
       <c r="M70" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="N70" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="N70" s="25" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:14">
@@ -4013,10 +4004,10 @@
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G71" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H71" s="22"/>
       <c r="I71" s="23"/>
@@ -4029,10 +4020,10 @@
         <v>47</v>
       </c>
       <c r="M71" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="N71" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="N71" s="25" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:14">
@@ -4047,10 +4038,10 @@
       </c>
       <c r="E72" s="20"/>
       <c r="F72" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G72" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H72" s="22"/>
       <c r="I72" s="23"/>
@@ -4063,10 +4054,10 @@
         <v>47</v>
       </c>
       <c r="M72" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="N72" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="N72" s="25" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="73" spans="1:14">
@@ -4081,10 +4072,10 @@
       </c>
       <c r="E73" s="20"/>
       <c r="F73" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G73" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H73" s="22"/>
       <c r="I73" s="23"/>
@@ -4097,10 +4088,10 @@
         <v>47</v>
       </c>
       <c r="M73" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="N73" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="N73" s="25" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -4118,10 +4109,10 @@
       </c>
       <c r="E74" s="20"/>
       <c r="F74" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G74" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H74" s="22"/>
       <c r="I74" s="23"/>
@@ -4134,10 +4125,10 @@
         <v>47</v>
       </c>
       <c r="M74" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N74" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="75" spans="1:14">
@@ -4145,7 +4136,7 @@
         <v>102</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>103</v>
@@ -4155,10 +4146,10 @@
       </c>
       <c r="E75" s="20"/>
       <c r="F75" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G75" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H75" s="22"/>
       <c r="I75" s="23"/>
@@ -4171,10 +4162,10 @@
         <v>47</v>
       </c>
       <c r="M75" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N75" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:14">
@@ -4192,10 +4183,10 @@
       </c>
       <c r="E76" s="20"/>
       <c r="F76" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G76" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H76" s="22"/>
       <c r="I76" s="23"/>
@@ -4208,10 +4199,10 @@
         <v>47</v>
       </c>
       <c r="M76" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N76" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="77" spans="1:14">
@@ -4229,10 +4220,10 @@
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G77" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H77" s="22"/>
       <c r="I77" s="23"/>
@@ -4245,10 +4236,10 @@
         <v>47</v>
       </c>
       <c r="M77" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N77" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -4266,10 +4257,10 @@
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G78" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H78" s="22"/>
       <c r="I78" s="23"/>
@@ -4282,10 +4273,10 @@
         <v>47</v>
       </c>
       <c r="M78" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N78" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -4303,10 +4294,10 @@
       </c>
       <c r="E79" s="20"/>
       <c r="F79" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G79" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H79" s="22"/>
       <c r="I79" s="23"/>
@@ -4319,10 +4310,10 @@
         <v>47</v>
       </c>
       <c r="M79" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N79" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -4340,10 +4331,10 @@
       </c>
       <c r="E80" s="20"/>
       <c r="F80" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G80" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H80" s="22"/>
       <c r="I80" s="23"/>
@@ -4356,10 +4347,10 @@
         <v>47</v>
       </c>
       <c r="M80" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N80" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:14">
@@ -4377,10 +4368,10 @@
       </c>
       <c r="E81" s="20"/>
       <c r="F81" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G81" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H81" s="22"/>
       <c r="I81" s="23"/>
@@ -4393,10 +4384,10 @@
         <v>47</v>
       </c>
       <c r="M81" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N81" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:14">
@@ -4414,10 +4405,10 @@
       </c>
       <c r="E82" s="20"/>
       <c r="F82" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G82" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H82" s="22"/>
       <c r="I82" s="23"/>
@@ -4430,10 +4421,10 @@
         <v>47</v>
       </c>
       <c r="M82" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N82" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:14">
@@ -4451,10 +4442,10 @@
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G83" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H83" s="22"/>
       <c r="I83" s="23"/>
@@ -4467,10 +4458,10 @@
         <v>47</v>
       </c>
       <c r="M83" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N83" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="84" spans="1:14">
@@ -4488,10 +4479,10 @@
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G84" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H84" s="22"/>
       <c r="I84" s="23"/>
@@ -4504,10 +4495,10 @@
         <v>47</v>
       </c>
       <c r="M84" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N84" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:14">
@@ -4525,10 +4516,10 @@
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G85" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H85" s="22"/>
       <c r="I85" s="23"/>
@@ -4541,10 +4532,10 @@
         <v>47</v>
       </c>
       <c r="M85" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N85" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86" spans="1:14">
@@ -4562,10 +4553,10 @@
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G86" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H86" s="22"/>
       <c r="I86" s="23"/>
@@ -4578,10 +4569,10 @@
         <v>47</v>
       </c>
       <c r="M86" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N86" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="87" spans="1:14">
@@ -4595,16 +4586,16 @@
         <v>103</v>
       </c>
       <c r="D87" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E87" s="46" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F87" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G87" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H87" s="22"/>
       <c r="I87" s="23">
@@ -4619,10 +4610,10 @@
         <v>47</v>
       </c>
       <c r="M87" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N87" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="1:14">
@@ -4636,16 +4627,16 @@
         <v>103</v>
       </c>
       <c r="D88" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E88" s="46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F88" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G88" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H88" s="22"/>
       <c r="I88" s="23">
@@ -4660,10 +4651,10 @@
         <v>47</v>
       </c>
       <c r="M88" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N88" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="1:14">
@@ -4677,16 +4668,16 @@
         <v>103</v>
       </c>
       <c r="D89" s="47" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E89" s="46" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F89" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G89" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H89" s="22"/>
       <c r="I89" s="23">
@@ -4701,10 +4692,10 @@
         <v>47</v>
       </c>
       <c r="M89" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N89" s="25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="90" spans="1:14">
@@ -4712,7 +4703,7 @@
         <v>121</v>
       </c>
       <c r="B90" s="46" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>103</v>
@@ -4721,13 +4712,13 @@
         <v>105</v>
       </c>
       <c r="E90" s="46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F90" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G90" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H90" s="22"/>
       <c r="I90" s="23">
@@ -4745,10 +4736,10 @@
         <v>47</v>
       </c>
       <c r="M90" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="N90" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="N90" s="25" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:14">
@@ -4756,7 +4747,7 @@
         <v>122</v>
       </c>
       <c r="B91" s="46" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C91" s="47" t="s">
         <v>103</v>
@@ -4765,13 +4756,13 @@
         <v>105</v>
       </c>
       <c r="E91" s="46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F91" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G91" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H91" s="22"/>
       <c r="I91" s="23">
@@ -4789,10 +4780,10 @@
         <v>47</v>
       </c>
       <c r="M91" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="N91" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="N91" s="25" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="92" spans="1:14">
@@ -4800,22 +4791,22 @@
         <v>123</v>
       </c>
       <c r="B92" s="46" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C92" s="47" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E92" s="46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F92" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H92" s="22"/>
       <c r="I92" s="23">
@@ -4833,10 +4824,10 @@
         <v>47</v>
       </c>
       <c r="M92" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="N92" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="N92" s="25" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="93" spans="1:14">
@@ -4844,22 +4835,22 @@
         <v>124</v>
       </c>
       <c r="B93" s="46" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C93" s="47" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E93" s="46" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F93" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G93" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H93" s="22"/>
       <c r="I93" s="23">
@@ -4877,10 +4868,10 @@
         <v>47</v>
       </c>
       <c r="M93" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="N93" s="25" t="s">
         <v>127</v>
-      </c>
-      <c r="N93" s="25" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:14">
@@ -4888,20 +4879,20 @@
         <v>125</v>
       </c>
       <c r="B94" s="46" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C94" s="47" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D94" s="47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E94" s="20"/>
       <c r="F94" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G94" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H94" s="22"/>
       <c r="I94" s="23">
@@ -4918,10 +4909,10 @@
         <v>47</v>
       </c>
       <c r="M94" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N94" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:14">
@@ -4929,20 +4920,20 @@
         <v>126</v>
       </c>
       <c r="B95" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C95" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="C95" s="47" t="s">
-        <v>200</v>
-      </c>
       <c r="D95" s="47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E95" s="20"/>
       <c r="F95" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G95" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H95" s="22"/>
       <c r="I95" s="23">
@@ -4959,10 +4950,10 @@
         <v>47</v>
       </c>
       <c r="M95" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N95" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="1:14">
@@ -4970,20 +4961,20 @@
         <v>127</v>
       </c>
       <c r="B96" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="C96" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="C96" s="47" t="s">
-        <v>201</v>
-      </c>
       <c r="D96" s="47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E96" s="20"/>
       <c r="F96" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G96" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H96" s="22"/>
       <c r="I96" s="23">
@@ -5000,10 +4991,10 @@
         <v>47</v>
       </c>
       <c r="M96" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N96" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="1:14">
@@ -5011,20 +5002,20 @@
         <v>128</v>
       </c>
       <c r="B97" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="C97" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="D97" s="47" t="s">
         <v>199</v>
-      </c>
-      <c r="C97" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="D97" s="47" t="s">
-        <v>202</v>
       </c>
       <c r="E97" s="20"/>
       <c r="F97" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G97" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H97" s="22"/>
       <c r="I97" s="23">
@@ -5041,10 +5032,10 @@
         <v>47</v>
       </c>
       <c r="M97" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N97" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -5052,22 +5043,22 @@
         <v>129</v>
       </c>
       <c r="B98" s="46" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C98" s="47" t="s">
+        <v>197</v>
+      </c>
+      <c r="D98" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="D98" s="47" t="s">
-        <v>203</v>
-      </c>
       <c r="E98" s="46" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F98" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G98" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H98" s="22"/>
       <c r="I98" s="23">
@@ -5084,10 +5075,10 @@
         <v>47</v>
       </c>
       <c r="M98" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N98" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -5095,22 +5086,22 @@
         <v>130</v>
       </c>
       <c r="B99" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="C99" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="C99" s="47" t="s">
+      <c r="D99" s="47" t="s">
         <v>200</v>
       </c>
-      <c r="D99" s="47" t="s">
-        <v>203</v>
-      </c>
       <c r="E99" s="46" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F99" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G99" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H99" s="22"/>
       <c r="I99" s="23">
@@ -5127,10 +5118,10 @@
         <v>47</v>
       </c>
       <c r="M99" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N99" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:14">
@@ -5138,22 +5129,22 @@
         <v>131</v>
       </c>
       <c r="B100" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="C100" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="C100" s="47" t="s">
+      <c r="D100" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="E100" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="D100" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="E100" s="46" t="s">
-        <v>204</v>
-      </c>
       <c r="F100" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G100" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H100" s="22"/>
       <c r="I100" s="23">
@@ -5170,10 +5161,10 @@
         <v>47</v>
       </c>
       <c r="M100" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N100" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="101" spans="1:14">
@@ -5181,22 +5172,22 @@
         <v>132</v>
       </c>
       <c r="B101" s="46" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C101" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="D101" s="47" t="s">
+        <v>200</v>
+      </c>
+      <c r="E101" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="D101" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="E101" s="46" t="s">
-        <v>204</v>
-      </c>
       <c r="F101" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G101" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H101" s="22"/>
       <c r="I101" s="23">
@@ -5213,10 +5204,10 @@
         <v>47</v>
       </c>
       <c r="M101" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N101" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="102" spans="1:14">
@@ -5228,10 +5219,10 @@
       </c>
       <c r="E102" s="20"/>
       <c r="F102" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G102" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H102" s="22"/>
       <c r="I102" s="23"/>
@@ -5245,268 +5236,276 @@
       </c>
       <c r="M102" s="20"/>
       <c r="N102" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="103" spans="1:14">
       <c r="A103" s="3">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B103" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E103" s="20"/>
+        <v>149</v>
+      </c>
+      <c r="C103" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D103" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E103" s="48" t="s">
+        <v>177</v>
+      </c>
       <c r="F103" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G103" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H103" s="22"/>
-      <c r="I103" s="23"/>
+      <c r="I103" s="3">
+        <v>298</v>
+      </c>
       <c r="J103" s="19">
-        <v>1360000000000</v>
+        <f>341*9807000</f>
+        <v>3344187000</v>
       </c>
       <c r="K103" s="19"/>
       <c r="L103" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M103" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="N103" s="27" t="s">
         <v>130</v>
-      </c>
-      <c r="N103" s="29" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="104" spans="1:14">
       <c r="A104" s="3">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B104" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C104" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D104" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E104" s="48" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F104" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G104" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H104" s="22"/>
       <c r="I104" s="3">
         <v>298</v>
       </c>
       <c r="J104" s="19">
-        <f>341*9807000</f>
-        <v>3344187000</v>
+        <f>338*9807000</f>
+        <v>3314766000</v>
       </c>
       <c r="K104" s="19"/>
       <c r="L104" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M104" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N104" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:14">
       <c r="A105" s="3">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C105" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D105" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E105" s="48" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F105" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G105" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H105" s="22"/>
       <c r="I105" s="3">
         <v>298</v>
       </c>
       <c r="J105" s="19">
-        <f>338*9807000</f>
-        <v>3314766000</v>
+        <f>340*9807000</f>
+        <v>3334380000</v>
       </c>
       <c r="K105" s="19"/>
       <c r="L105" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M105" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N105" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:14">
       <c r="A106" s="3">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B106" s="30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C106" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D106" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E106" s="48" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F106" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G106" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H106" s="22"/>
       <c r="I106" s="3">
         <v>298</v>
       </c>
       <c r="J106" s="19">
-        <f>340*9807000</f>
-        <v>3334380000</v>
+        <f>345*9807000</f>
+        <v>3383415000</v>
       </c>
       <c r="K106" s="19"/>
       <c r="L106" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M106" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N106" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="1:14">
       <c r="A107" s="3">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B107" s="30" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C107" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D107" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E107" s="48" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F107" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G107" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H107" s="22"/>
       <c r="I107" s="3">
         <v>298</v>
       </c>
       <c r="J107" s="19">
-        <f>345*9807000</f>
-        <v>3383415000</v>
+        <f>334*9807000</f>
+        <v>3275538000</v>
       </c>
       <c r="K107" s="19"/>
       <c r="L107" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M107" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N107" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="108" spans="1:14">
       <c r="A108" s="3">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B108" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C108" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D108" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E108" s="48" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F108" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G108" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H108" s="22"/>
       <c r="I108" s="3">
         <v>298</v>
       </c>
       <c r="J108" s="19">
-        <f>334*9807000</f>
-        <v>3275538000</v>
+        <f>340*9807000</f>
+        <v>3334380000</v>
       </c>
       <c r="K108" s="19"/>
       <c r="L108" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M108" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N108" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="109" spans="1:14">
       <c r="A109" s="3">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C109" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D109" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E109" s="48" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F109" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G109" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H109" s="22"/>
       <c r="I109" s="3">
@@ -5521,314 +5520,314 @@
         <v>47</v>
       </c>
       <c r="M109" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N109" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="1:14">
       <c r="A110" s="3">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C110" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D110" s="34" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E110" s="48" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="F110" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G110" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H110" s="22"/>
       <c r="I110" s="3">
         <v>298</v>
       </c>
       <c r="J110" s="19">
-        <f>340*9807000</f>
-        <v>3334380000</v>
+        <f>331*9807000</f>
+        <v>3246117000</v>
       </c>
       <c r="K110" s="19"/>
       <c r="L110" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M110" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N110" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:14">
       <c r="A111" s="3">
-        <v>142</v>
-      </c>
-      <c r="B111" s="30" t="s">
-        <v>155</v>
+        <v>143</v>
+      </c>
+      <c r="B111" s="46" t="s">
+        <v>203</v>
       </c>
       <c r="C111" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="D111" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="E111" s="48" t="s">
-        <v>181</v>
+      <c r="D111" s="47" t="s">
+        <v>204</v>
       </c>
       <c r="F111" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G111" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H111" s="22"/>
       <c r="I111" s="3">
         <v>298</v>
       </c>
       <c r="J111" s="19">
-        <f>331*9807000</f>
-        <v>3246117000</v>
+        <f>459*9807000</f>
+        <v>4501413000</v>
       </c>
       <c r="K111" s="19"/>
       <c r="L111" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M111" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="N111" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="N111" s="29" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="3">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B112" s="46" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C112" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D112" s="47" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="E112" s="46" t="s">
+        <v>206</v>
       </c>
       <c r="F112" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G112" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H112" s="22"/>
       <c r="I112" s="3">
         <v>298</v>
       </c>
       <c r="J112" s="19">
-        <f>459*9807000</f>
-        <v>4501413000</v>
+        <f>487*9807000</f>
+        <v>4776009000</v>
       </c>
       <c r="K112" s="19"/>
       <c r="L112" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M112" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N112" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:14">
       <c r="A113" s="3">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B113" s="46" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C113" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D113" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="E113" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="E113" s="46" t="s">
-        <v>209</v>
-      </c>
       <c r="F113" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G113" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H113" s="22"/>
       <c r="I113" s="3">
         <v>298</v>
       </c>
       <c r="J113" s="19">
-        <f>487*9807000</f>
-        <v>4776009000</v>
+        <f>456*9807000</f>
+        <v>4471992000</v>
       </c>
       <c r="K113" s="19"/>
       <c r="L113" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M113" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N113" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="114" spans="1:14">
       <c r="A114" s="3">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B114" s="46" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C114" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D114" s="47" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E114" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F114" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G114" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H114" s="22"/>
       <c r="I114" s="3">
         <v>298</v>
       </c>
       <c r="J114" s="19">
-        <f>456*9807000</f>
-        <v>4471992000</v>
+        <f>516*9807000</f>
+        <v>5060412000</v>
       </c>
       <c r="K114" s="19"/>
       <c r="L114" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M114" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N114" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="115" spans="1:14">
       <c r="A115" s="3">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B115" s="46" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C115" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D115" s="47" t="s">
-        <v>210</v>
-      </c>
-      <c r="E115" s="46" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="F115" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G115" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H115" s="22"/>
       <c r="I115" s="3">
         <v>298</v>
       </c>
       <c r="J115" s="19">
-        <f>516*9807000</f>
-        <v>5060412000</v>
+        <f>445*9807000</f>
+        <v>4364115000</v>
       </c>
       <c r="K115" s="19"/>
       <c r="L115" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M115" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N115" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="116" spans="1:14">
       <c r="A116" s="3">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B116" s="46" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C116" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D116" s="47" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="E116" s="46" t="s">
+        <v>206</v>
       </c>
       <c r="F116" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G116" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H116" s="22"/>
       <c r="I116" s="3">
         <v>298</v>
       </c>
       <c r="J116" s="19">
-        <f>445*9807000</f>
-        <v>4364115000</v>
+        <f>459*9807000</f>
+        <v>4501413000</v>
       </c>
       <c r="K116" s="19"/>
       <c r="L116" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M116" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N116" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="117" spans="1:14">
       <c r="A117" s="3">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B117" s="46" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C117" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D117" s="47" t="s">
+        <v>207</v>
+      </c>
+      <c r="E117" s="46" t="s">
         <v>208</v>
       </c>
-      <c r="E117" s="46" t="s">
-        <v>209</v>
-      </c>
       <c r="F117" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G117" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H117" s="22"/>
       <c r="I117" s="3">
@@ -5843,293 +5842,298 @@
         <v>47</v>
       </c>
       <c r="M117" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N117" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="118" spans="1:14">
       <c r="A118" s="3">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B118" s="46" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C118" s="47" t="s">
         <v>103</v>
       </c>
       <c r="D118" s="47" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E118" s="46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F118" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G118" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H118" s="22"/>
       <c r="I118" s="3">
         <v>298</v>
       </c>
       <c r="J118" s="19">
-        <f>459*9807000</f>
-        <v>4501413000</v>
+        <f>522*9807000</f>
+        <v>5119254000</v>
       </c>
       <c r="K118" s="19"/>
       <c r="L118" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M118" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="N118" s="29" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="119" spans="1:14">
       <c r="A119" s="3">
-        <v>150</v>
-      </c>
-      <c r="B119" s="46" t="s">
-        <v>205</v>
-      </c>
-      <c r="C119" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B119" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D119" s="47" t="s">
-        <v>210</v>
-      </c>
-      <c r="E119" s="46" t="s">
-        <v>212</v>
-      </c>
+      <c r="E119" s="20"/>
       <c r="F119" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G119" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H119" s="22"/>
-      <c r="I119" s="3">
-        <v>298</v>
-      </c>
+      <c r="I119" s="23"/>
       <c r="J119" s="19">
-        <f>522*9807000</f>
-        <v>5119254000</v>
+        <f>960*9807000</f>
+        <v>9414720000</v>
       </c>
       <c r="K119" s="19"/>
       <c r="L119" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M119" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="N119" s="29" t="s">
         <v>133</v>
-      </c>
-      <c r="N119" s="29" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="120" spans="1:14">
       <c r="A120" s="3">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B120" s="20" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E120" s="20"/>
       <c r="F120" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G120" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H120" s="22"/>
       <c r="I120" s="23"/>
       <c r="J120" s="19">
-        <f>960*9807000</f>
-        <v>9414720000</v>
+        <f>920*9807000</f>
+        <v>9022440000</v>
       </c>
       <c r="K120" s="19"/>
       <c r="L120" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M120" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="N120" s="29" t="s">
         <v>133</v>
-      </c>
-      <c r="N120" s="29" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="121" spans="1:14">
       <c r="A121" s="3">
-        <v>152</v>
-      </c>
-      <c r="B121" s="20" t="s">
-        <v>100</v>
+        <v>153</v>
+      </c>
+      <c r="B121" s="30" t="s">
+        <v>135</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E121" s="20"/>
       <c r="F121" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G121" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H121" s="22"/>
       <c r="I121" s="23"/>
       <c r="J121" s="19">
-        <f>920*9807000</f>
-        <v>9022440000</v>
+        <f>830*9807000</f>
+        <v>8139810000</v>
       </c>
       <c r="K121" s="19"/>
       <c r="L121" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M121" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="N121" s="29" t="s">
         <v>133</v>
-      </c>
-      <c r="N121" s="29" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="122" spans="1:14">
       <c r="A122" s="3">
-        <v>153</v>
-      </c>
-      <c r="B122" s="30" t="s">
-        <v>137</v>
+        <v>154</v>
+      </c>
+      <c r="B122" s="20" t="s">
+        <v>101</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E122" s="20"/>
       <c r="F122" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G122" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H122" s="22"/>
       <c r="I122" s="23"/>
       <c r="J122" s="19">
-        <f>830*9807000</f>
-        <v>8139810000</v>
+        <f>840*9807000</f>
+        <v>8237880000</v>
       </c>
       <c r="K122" s="19"/>
       <c r="L122" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M122" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="N122" s="29" t="s">
         <v>133</v>
-      </c>
-      <c r="N122" s="29" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="123" spans="1:14">
       <c r="A123" s="3">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B123" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E123" s="20"/>
       <c r="F123" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G123" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H123" s="22"/>
       <c r="I123" s="23"/>
       <c r="J123" s="19">
-        <f>840*9807000</f>
-        <v>8237880000</v>
+        <f>850*9807000</f>
+        <v>8335950000</v>
       </c>
       <c r="K123" s="19"/>
       <c r="L123" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M123" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="N123" s="29" t="s">
         <v>133</v>
-      </c>
-      <c r="N123" s="29" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="124" spans="1:14">
       <c r="A124" s="3">
-        <v>155</v>
-      </c>
-      <c r="B124" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="C124" s="3" t="s">
-        <v>103</v>
+        <v>156</v>
+      </c>
+      <c r="B124" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="C124" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="D124" s="47" t="s">
+        <v>199</v>
       </c>
       <c r="E124" s="20"/>
       <c r="F124" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G124" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H124" s="22"/>
-      <c r="I124" s="23"/>
+        <v>106</v>
+      </c>
+      <c r="H124" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="I124" s="23">
+        <v>298</v>
+      </c>
       <c r="J124" s="19">
-        <f>850*9807000</f>
-        <v>8335950000</v>
-      </c>
-      <c r="K124" s="19"/>
+        <f>829*9807000</f>
+        <v>8130003000</v>
+      </c>
+      <c r="K124" s="19">
+        <f>1*9807000</f>
+        <v>9807000</v>
+      </c>
       <c r="L124" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M124" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="N124" s="29" t="s">
-        <v>135</v>
+        <v>115</v>
+      </c>
+      <c r="N124" s="25" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="125" spans="1:14">
       <c r="A125" s="3">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B125" s="46" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C125" s="47" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D125" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="E125" s="20"/>
+        <v>211</v>
+      </c>
+      <c r="E125" s="46" t="s">
+        <v>212</v>
+      </c>
       <c r="F125" s="30" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G125" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H125" s="49" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="I125" s="23">
         <v>298</v>
       </c>
       <c r="J125" s="19">
-        <f>829*9807000</f>
-        <v>8130003000</v>
+        <f>920*9807000</f>
+        <v>9022440000</v>
       </c>
       <c r="K125" s="19">
         <f>1*9807000</f>
@@ -6139,89 +6143,89 @@
         <v>47</v>
       </c>
       <c r="M125" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N125" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="126" spans="1:14">
       <c r="A126" s="3">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B126" s="46" t="s">
+        <v>210</v>
+      </c>
+      <c r="C126" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="D126" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="E126" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="C126" s="47" t="s">
-        <v>219</v>
-      </c>
-      <c r="D126" s="47" t="s">
+      <c r="F126" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="G126" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H126" s="49" t="s">
         <v>214</v>
-      </c>
-      <c r="E126" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="F126" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="G126" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H126" s="49" t="s">
-        <v>217</v>
       </c>
       <c r="I126" s="23">
         <v>298</v>
       </c>
       <c r="J126" s="19">
-        <f>920*9807000</f>
-        <v>9022440000</v>
+        <f>931*9807000</f>
+        <v>9130317000</v>
       </c>
       <c r="K126" s="19">
-        <f>1*9807000</f>
-        <v>9807000</v>
+        <f>2*9807000</f>
+        <v>19614000</v>
       </c>
       <c r="L126" s="20" t="s">
         <v>47</v>
       </c>
       <c r="M126" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N126" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="127" spans="1:14">
       <c r="A127" s="3">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B127" s="46" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C127" s="47" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D127" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="E127" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="F127" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="G127" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="H127" s="49" t="s">
         <v>214</v>
-      </c>
-      <c r="E127" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="F127" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="G127" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H127" s="49" t="s">
-        <v>217</v>
       </c>
       <c r="I127" s="23">
         <v>298</v>
       </c>
       <c r="J127" s="19">
-        <f>931*9807000</f>
-        <v>9130317000</v>
+        <f>960*9807000</f>
+        <v>9414720000</v>
       </c>
       <c r="K127" s="19">
         <f>2*9807000</f>
@@ -6231,57 +6235,21 @@
         <v>47</v>
       </c>
       <c r="M127" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N127" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="128" spans="1:14">
-      <c r="A128" s="3">
-        <v>159</v>
-      </c>
-      <c r="B128" s="46" t="s">
-        <v>213</v>
-      </c>
-      <c r="C128" s="47" t="s">
-        <v>219</v>
-      </c>
-      <c r="D128" s="47" t="s">
-        <v>214</v>
-      </c>
-      <c r="E128" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="F128" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="G128" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H128" s="49" t="s">
-        <v>217</v>
-      </c>
-      <c r="I128" s="23">
-        <v>298</v>
-      </c>
-      <c r="J128" s="19">
-        <f>960*9807000</f>
-        <v>9414720000</v>
-      </c>
-      <c r="K128" s="19">
-        <f>2*9807000</f>
-        <v>19614000</v>
-      </c>
-      <c r="L128" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="M128" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="N128" s="25" t="s">
-        <v>136</v>
-      </c>
+      <c r="E128" s="20"/>
+      <c r="F128" s="30"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="22"/>
+      <c r="I128" s="23"/>
+      <c r="K128" s="19"/>
+      <c r="L128" s="30"/>
+      <c r="M128" s="20"/>
     </row>
     <row r="129" spans="5:13">
       <c r="E129" s="20"/>
@@ -6464,8 +6432,9 @@
       <c r="M146" s="20"/>
     </row>
     <row r="147" spans="4:13">
+      <c r="D147" s="22"/>
       <c r="E147" s="20"/>
-      <c r="F147" s="30"/>
+      <c r="F147" s="31"/>
       <c r="G147" s="20"/>
       <c r="H147" s="22"/>
       <c r="I147" s="23"/>
@@ -6936,15 +6905,20 @@
       <c r="M189" s="20"/>
     </row>
     <row r="190" spans="1:14">
+      <c r="A190" s="24"/>
+      <c r="B190" s="20"/>
+      <c r="C190" s="22"/>
       <c r="D190" s="22"/>
       <c r="E190" s="20"/>
-      <c r="F190" s="31"/>
-      <c r="G190" s="20"/>
+      <c r="F190" s="22"/>
+      <c r="G190" s="22"/>
       <c r="H190" s="22"/>
       <c r="I190" s="23"/>
+      <c r="J190" s="19"/>
       <c r="K190" s="19"/>
-      <c r="L190" s="30"/>
+      <c r="L190" s="20"/>
       <c r="M190" s="20"/>
+      <c r="N190" s="25"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="24"/>
@@ -6960,7 +6934,6 @@
       <c r="K191" s="19"/>
       <c r="L191" s="20"/>
       <c r="M191" s="20"/>
-      <c r="N191" s="25"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="24"/>
@@ -7066,6 +7039,7 @@
       <c r="K198" s="19"/>
       <c r="L198" s="20"/>
       <c r="M198" s="20"/>
+      <c r="N198" s="25"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="24"/>
@@ -7081,7 +7055,6 @@
       <c r="K199" s="19"/>
       <c r="L199" s="20"/>
       <c r="M199" s="20"/>
-      <c r="N199" s="25"/>
     </row>
     <row r="200" spans="1:14">
       <c r="A200" s="24"/>
@@ -7187,6 +7160,7 @@
       <c r="K206" s="19"/>
       <c r="L206" s="20"/>
       <c r="M206" s="20"/>
+      <c r="N206" s="25"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="24"/>
@@ -7522,7 +7496,7 @@
       <c r="K227" s="19"/>
       <c r="L227" s="20"/>
       <c r="M227" s="20"/>
-      <c r="N227" s="25"/>
+      <c r="N227" s="27"/>
     </row>
     <row r="228" spans="1:14">
       <c r="A228" s="24"/>
@@ -7637,14 +7611,13 @@
       <c r="N234" s="27"/>
     </row>
     <row r="235" spans="1:14">
-      <c r="A235" s="24"/>
+      <c r="A235" s="11"/>
       <c r="B235" s="20"/>
-      <c r="C235" s="22"/>
-      <c r="D235" s="22"/>
-      <c r="E235" s="20"/>
-      <c r="F235" s="22"/>
-      <c r="G235" s="22"/>
-      <c r="H235" s="22"/>
+      <c r="C235" s="5"/>
+      <c r="D235" s="5"/>
+      <c r="F235" s="5"/>
+      <c r="G235" s="5"/>
+      <c r="H235" s="5"/>
       <c r="I235" s="23"/>
       <c r="J235" s="19"/>
       <c r="K235" s="19"/>
@@ -7695,7 +7668,7 @@
       <c r="K238" s="19"/>
       <c r="L238" s="20"/>
       <c r="M238" s="20"/>
-      <c r="N238" s="27"/>
+      <c r="N238" s="25"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="11"/>
@@ -7935,7 +7908,7 @@
       <c r="K254" s="19"/>
       <c r="L254" s="20"/>
       <c r="M254" s="20"/>
-      <c r="N254" s="25"/>
+      <c r="N254" s="28"/>
     </row>
     <row r="255" spans="1:14">
       <c r="A255" s="11"/>
@@ -7995,7 +7968,7 @@
       <c r="K258" s="19"/>
       <c r="L258" s="20"/>
       <c r="M258" s="20"/>
-      <c r="N258" s="28"/>
+      <c r="N258" s="25"/>
     </row>
     <row r="259" spans="1:14">
       <c r="A259" s="11"/>
@@ -8160,7 +8133,7 @@
       <c r="K269" s="19"/>
       <c r="L269" s="20"/>
       <c r="M269" s="20"/>
-      <c r="N269" s="25"/>
+      <c r="N269" s="29"/>
     </row>
     <row r="270" spans="1:14">
       <c r="A270" s="11"/>
@@ -8205,7 +8178,7 @@
       <c r="K272" s="19"/>
       <c r="L272" s="20"/>
       <c r="M272" s="20"/>
-      <c r="N272" s="29"/>
+      <c r="N272" s="27"/>
     </row>
     <row r="273" spans="1:14">
       <c r="A273" s="11"/>
@@ -8325,7 +8298,7 @@
       <c r="K280" s="19"/>
       <c r="L280" s="20"/>
       <c r="M280" s="20"/>
-      <c r="N280" s="27"/>
+      <c r="N280" s="29"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="11"/>
@@ -8343,7 +8316,6 @@
       <c r="N281" s="29"/>
     </row>
     <row r="282" spans="1:14">
-      <c r="A282" s="11"/>
       <c r="B282" s="20"/>
       <c r="C282" s="5"/>
       <c r="D282" s="5"/>
@@ -8509,7 +8481,7 @@
       <c r="K293" s="19"/>
       <c r="L293" s="20"/>
       <c r="M293" s="20"/>
-      <c r="N293" s="29"/>
+      <c r="N293" s="25"/>
     </row>
     <row r="294" spans="2:14">
       <c r="B294" s="20"/>
@@ -8554,18 +8526,17 @@
       <c r="N296" s="25"/>
     </row>
     <row r="297" spans="2:14">
-      <c r="B297" s="20"/>
       <c r="C297" s="5"/>
       <c r="D297" s="5"/>
       <c r="F297" s="5"/>
       <c r="G297" s="5"/>
       <c r="H297" s="5"/>
-      <c r="I297" s="23"/>
+      <c r="I297" s="18"/>
       <c r="J297" s="19"/>
       <c r="K297" s="19"/>
       <c r="L297" s="20"/>
       <c r="M297" s="20"/>
-      <c r="N297" s="25"/>
+      <c r="N297" s="20"/>
     </row>
     <row r="298" spans="2:14">
       <c r="C298" s="5"/>
@@ -9983,19 +9954,6 @@
       <c r="L406" s="20"/>
       <c r="M406" s="20"/>
       <c r="N406" s="20"/>
-    </row>
-    <row r="407" spans="3:14">
-      <c r="C407" s="5"/>
-      <c r="D407" s="5"/>
-      <c r="F407" s="5"/>
-      <c r="G407" s="5"/>
-      <c r="H407" s="5"/>
-      <c r="I407" s="18"/>
-      <c r="J407" s="19"/>
-      <c r="K407" s="19"/>
-      <c r="L407" s="20"/>
-      <c r="M407" s="20"/>
-      <c r="N407" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="19">

</xml_diff>

<commit_message>
- fixed incorrectly reported property values from `10.1016/j.msea.2016.07.102`
</commit_message>
<xml_diff>
--- a/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
+++ b/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55D0ECB-2AA6-234E-B289-CEFA9D346814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53FFE20-0286-F740-92BB-DE2F8BC4BA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9300" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1337,8 +1337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T406"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -3108,7 +3108,8 @@
         <v>298</v>
       </c>
       <c r="J47" s="19">
-        <v>609</v>
+        <f>609*9807000</f>
+        <v>5972463000</v>
       </c>
       <c r="K47" s="19"/>
       <c r="L47" s="20" t="s">
@@ -3143,7 +3144,8 @@
         <v>298</v>
       </c>
       <c r="J48" s="19">
-        <v>1320000000</v>
+        <f>1320*9807000</f>
+        <v>12945240000</v>
       </c>
       <c r="K48" s="19"/>
       <c r="L48" s="20" t="s">
@@ -3178,7 +3180,8 @@
         <v>298</v>
       </c>
       <c r="J49" s="19">
-        <v>873000000</v>
+        <f>873*9807000</f>
+        <v>8561511000</v>
       </c>
       <c r="K49" s="19"/>
       <c r="L49" s="20" t="s">
@@ -3213,7 +3216,8 @@
         <v>298</v>
       </c>
       <c r="J50" s="19">
-        <v>970000000</v>
+        <f>970*9807000</f>
+        <v>9512790000</v>
       </c>
       <c r="K50" s="19"/>
       <c r="L50" s="20" t="s">
@@ -3248,7 +3252,8 @@
         <v>298</v>
       </c>
       <c r="J51" s="19">
-        <v>628000000</v>
+        <f>628*9807000</f>
+        <v>6158796000</v>
       </c>
       <c r="K51" s="19"/>
       <c r="L51" s="20" t="s">
@@ -3283,7 +3288,8 @@
         <v>298</v>
       </c>
       <c r="J52" s="19">
-        <v>3430000000</v>
+        <f>3430*9807000</f>
+        <v>33638010000</v>
       </c>
       <c r="K52" s="19"/>
       <c r="L52" s="20" t="s">
@@ -3318,9 +3324,13 @@
         <v>298</v>
       </c>
       <c r="J53" s="19">
-        <v>3113000000</v>
-      </c>
-      <c r="K53" s="19"/>
+        <f>3113*9807000</f>
+        <v>30529191000</v>
+      </c>
+      <c r="K53" s="19">
+        <f>46*9807000</f>
+        <v>451122000</v>
+      </c>
       <c r="L53" s="20" t="s">
         <v>47</v>
       </c>
@@ -3353,9 +3363,13 @@
         <v>298</v>
       </c>
       <c r="J54" s="19">
-        <v>4830000000</v>
-      </c>
-      <c r="K54" s="19"/>
+        <f>4830*9807000</f>
+        <v>47367810000</v>
+      </c>
+      <c r="K54" s="19">
+        <f>29*9807000</f>
+        <v>284403000</v>
+      </c>
       <c r="L54" s="20" t="s">
         <v>47</v>
       </c>
@@ -3388,9 +3402,13 @@
         <v>298</v>
       </c>
       <c r="J55" s="19">
-        <v>4380000000</v>
-      </c>
-      <c r="K55" s="19"/>
+        <f>4380*9807000</f>
+        <v>42954660000</v>
+      </c>
+      <c r="K55" s="19">
+        <f>34*9807000</f>
+        <v>333438000</v>
+      </c>
       <c r="L55" s="20" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
- unit conversion bugfix in `10.1016/j.msea.2016.07.102`
</commit_message>
<xml_diff>
--- a/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
+++ b/MarciaAhn_Hardness_Nov2022_AdamFix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/VSCode Projects/ULTERA-contribute-guest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B6509-1D6E-AD47-BDDA-90DCDDC6BB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD90C81F-4BEA-254D-A195-2423AAD9A9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9300" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1029,6 +1029,16 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1047,16 +1057,6 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T406"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="86" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O113" sqref="O113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1382,21 +1382,21 @@
       <c r="B2" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
       <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1">
@@ -1406,17 +1406,17 @@
       <c r="B3" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1">
@@ -1434,43 +1434,43 @@
       <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="47" t="s">
+      <c r="K5" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="47" t="s">
+      <c r="L5" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="M5" s="47" t="s">
+      <c r="M5" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="N5" s="47" t="s">
+      <c r="N5" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="48" t="s">
+      <c r="O5" s="42" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1481,19 +1481,19 @@
       <c r="B6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="48"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="42"/>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" s="1" t="s">
@@ -1538,7 +1538,7 @@
       <c r="N7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="48"/>
+      <c r="O7" s="42"/>
       <c r="P7" s="9" t="s">
         <v>43</v>
       </c>
@@ -1551,35 +1551,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1">
       <c r="A8" s="11"/>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="45" t="s">
+      <c r="C8" s="48"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="46" t="s">
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="46"/>
+      <c r="N8" s="50"/>
       <c r="O8" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="49" t="s">
+      <c r="P8" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="49"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1">
       <c r="A9" s="5" t="s">
@@ -3152,8 +3152,8 @@
         <v>298</v>
       </c>
       <c r="J48" s="19">
-        <f>1320*9807000</f>
-        <v>12945240000</v>
+        <f>1320000000</f>
+        <v>1320000000</v>
       </c>
       <c r="K48" s="19"/>
       <c r="L48" s="20" t="s">
@@ -3188,8 +3188,8 @@
         <v>298</v>
       </c>
       <c r="J49" s="19">
-        <f>873*9807000</f>
-        <v>8561511000</v>
+        <f>873000000</f>
+        <v>873000000</v>
       </c>
       <c r="K49" s="19"/>
       <c r="L49" s="20" t="s">
@@ -3224,8 +3224,8 @@
         <v>298</v>
       </c>
       <c r="J50" s="19">
-        <f>970*9807000</f>
-        <v>9512790000</v>
+        <f>970000000</f>
+        <v>970000000</v>
       </c>
       <c r="K50" s="19"/>
       <c r="L50" s="20" t="s">
@@ -3260,8 +3260,8 @@
         <v>298</v>
       </c>
       <c r="J51" s="19">
-        <f>628*9807000</f>
-        <v>6158796000</v>
+        <f>628000000</f>
+        <v>628000000</v>
       </c>
       <c r="K51" s="19"/>
       <c r="L51" s="20" t="s">
@@ -3296,8 +3296,8 @@
         <v>298</v>
       </c>
       <c r="J52" s="19">
-        <f>3430*9807000</f>
-        <v>33638010000</v>
+        <f>3430000000</f>
+        <v>3430000000</v>
       </c>
       <c r="K52" s="19"/>
       <c r="L52" s="20" t="s">
@@ -3320,7 +3320,7 @@
       <c r="C53" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D53" s="50" t="s">
+      <c r="D53" s="41" t="s">
         <v>204</v>
       </c>
       <c r="E53" s="20"/>
@@ -3335,12 +3335,12 @@
         <v>298</v>
       </c>
       <c r="J53" s="19">
-        <f>3113*9807000</f>
-        <v>30529191000</v>
+        <f>3113000000</f>
+        <v>3113000000</v>
       </c>
       <c r="K53" s="19">
-        <f>46*9807000</f>
-        <v>451122000</v>
+        <f>46000000</f>
+        <v>46000000</v>
       </c>
       <c r="L53" s="20" t="s">
         <v>47</v>
@@ -3362,7 +3362,7 @@
       <c r="C54" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="50" t="s">
+      <c r="D54" s="41" t="s">
         <v>204</v>
       </c>
       <c r="E54" s="20"/>
@@ -3377,12 +3377,12 @@
         <v>298</v>
       </c>
       <c r="J54" s="19">
-        <f>4830*9807000</f>
-        <v>47367810000</v>
+        <f>4830000000</f>
+        <v>4830000000</v>
       </c>
       <c r="K54" s="19">
-        <f>29*9807000</f>
-        <v>284403000</v>
+        <f>29000000</f>
+        <v>29000000</v>
       </c>
       <c r="L54" s="20" t="s">
         <v>47</v>
@@ -3404,7 +3404,7 @@
       <c r="C55" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D55" s="50" t="s">
+      <c r="D55" s="41" t="s">
         <v>204</v>
       </c>
       <c r="E55" s="20"/>
@@ -3419,12 +3419,12 @@
         <v>298</v>
       </c>
       <c r="J55" s="19">
-        <f>4380*9807000</f>
-        <v>42954660000</v>
+        <f>4380000000</f>
+        <v>4380000000</v>
       </c>
       <c r="K55" s="19">
-        <f>34*9807000</f>
-        <v>333438000</v>
+        <f>34000000</f>
+        <v>34000000</v>
       </c>
       <c r="L55" s="20" t="s">
         <v>47</v>
@@ -9992,11 +9992,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -10011,6 +10006,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>

</xml_diff>